<commit_message>
Not sure if this is the right change to augmentation defaults
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="172">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -535,7 +535,14 @@
     <t>added</t>
   </si>
   <si>
-    <t>-network setup d n- fails if there's another n variable, even with trtlist() option correctly specified</t>
+    <t>-network setup d n- in wide format fails if there's another n variable, even with trtlist() option correctly specified</t>
+  </si>
+  <si>
+    <t>bug fixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defaults now augment(1E-5) in setup and  large(1E5) in convert.
+Notes added to help file </t>
   </si>
 </sst>
 </file>
@@ -1011,10 +1018,10 @@
   <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,8 +1273,12 @@
       <c r="D14" s="5">
         <v>42314</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14" s="7">
+        <v>43194</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1282,8 +1293,12 @@
       <c r="D15" s="5">
         <v>42388</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F15" s="7">
+        <v>43194</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">

</xml_diff>

<commit_message>
Minor improvements to setup, meta, forest, FAQs
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -11,7 +11,7 @@
     <sheet name="versions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$F$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$F$80</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'To do'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="174">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -438,9 +438,6 @@
     <t>fixed bug at l467</t>
   </si>
   <si>
-    <t>give advice to avoid underscore in treatment names</t>
-  </si>
-  <si>
     <t>Failure in the output for forest plot if network meta regresses on a constant one - as is useful with inf priors / pseudodata
 network meta c, reg(one) nocons collinear</t>
   </si>
@@ -543,6 +540,15 @@
   <si>
     <t xml:space="preserve">Defaults now augment(1E-5) in setup and  large(1E5) in convert.
 Notes added to help file </t>
+  </si>
+  <si>
+    <t>too late to be worth doing</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>not sure how to do this without making labels too long.</t>
   </si>
 </sst>
 </file>
@@ -659,12 +665,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1015,13 +1016,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,7 +1266,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>60</v>
@@ -1274,7 +1275,7 @@
         <v>42314</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F14" s="7">
         <v>43194</v>
@@ -1294,7 +1295,7 @@
         <v>42388</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F15" s="7">
         <v>43194</v>
@@ -1422,7 +1423,7 @@
         <v>42314</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F22" s="8">
         <v>42964</v>
@@ -1433,7 +1434,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>60</v>
@@ -1815,8 +1816,12 @@
       <c r="D46" s="5">
         <v>42619</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="7"/>
+      <c r="E46" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F46" s="7">
+        <v>43194</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
@@ -1843,7 +1848,7 @@
         <v>12</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>60</v>
@@ -1983,7 +1988,7 @@
         <v>15</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>60</v>
@@ -2211,8 +2216,12 @@
       <c r="D70" s="5">
         <v>42188</v>
       </c>
-      <c r="E70" s="4"/>
-      <c r="F70" s="7"/>
+      <c r="E70" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F70" s="7">
+        <v>43194</v>
+      </c>
     </row>
     <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
@@ -2227,8 +2236,12 @@
       <c r="D71" s="5">
         <v>42193</v>
       </c>
-      <c r="E71" s="4"/>
-      <c r="F71" s="7"/>
+      <c r="E71" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F71" s="7">
+        <v>42207</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
@@ -2243,10 +2256,14 @@
       <c r="D72" s="5">
         <v>42256</v>
       </c>
-      <c r="E72" s="4"/>
-      <c r="F72" s="7"/>
-    </row>
-    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E72" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F72" s="7">
+        <v>42380</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>22</v>
       </c>
@@ -2259,7 +2276,9 @@
       <c r="D73" s="5">
         <v>42472</v>
       </c>
-      <c r="E73" s="4"/>
+      <c r="E73" s="4" t="s">
+        <v>173</v>
+      </c>
       <c r="F73" s="7"/>
     </row>
     <row r="74" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -2317,8 +2336,12 @@
       <c r="D77" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E77" s="4"/>
-      <c r="F77" s="3"/>
+      <c r="E77" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F77" s="7">
+        <v>43194</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
@@ -2349,8 +2372,12 @@
       <c r="D79" s="5">
         <v>42205</v>
       </c>
-      <c r="E79" s="4"/>
-      <c r="F79" s="3"/>
+      <c r="E79" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F79" s="7">
+        <v>42207</v>
+      </c>
     </row>
     <row r="80" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
@@ -2365,70 +2392,53 @@
       <c r="D80" s="5">
         <v>42205</v>
       </c>
-      <c r="E80" s="4"/>
-      <c r="F80" s="3"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D81" s="5">
-        <v>42915</v>
-      </c>
-      <c r="E81" s="4"/>
-      <c r="F81" s="3"/>
+      <c r="E80" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F81"/>
+  <autoFilter ref="A2:F80"/>
   <conditionalFormatting sqref="B70:B78 B65:B68 B3:B13 B18:B22 B15:B16 B46:B55 B24:B44 B57:B63">
-    <cfRule type="expression" dxfId="10" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>ISBLANK($F3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>ISBLANK($F64)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>ISBLANK($F69)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>ISBLANK($F79)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>ISBLANK($F80)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>ISBLANK($F17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>ISBLANK($F14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>ISBLANK($F45)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B81">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>ISBLANK($F81)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
@@ -2468,67 +2478,67 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="M3" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q3" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2537,7 +2547,7 @@
       </c>
       <c r="C5" s="10"/>
       <c r="L5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -2546,36 +2556,36 @@
       </c>
       <c r="C6" s="12"/>
       <c r="P6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" s="10">
         <v>42976</v>
       </c>
       <c r="C8" s="10"/>
       <c r="P8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B9" s="10">
         <v>43017</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2586,15 +2596,15 @@
         <v>43105</v>
       </c>
       <c r="P10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enabled network bayes, model(#). Program still fails when run as in paper - about sigC vs sigC2 in model 1CB.
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -11,7 +11,7 @@
     <sheet name="versions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$F$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$F$85</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'To do'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="179">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -561,6 +561,9 @@
   </si>
   <si>
     <t>wrong output matrix with standard format - affects forest plot</t>
+  </si>
+  <si>
+    <t>Check error handling when importing multi-arm trials from pairs format if some contrasts are missing</t>
   </si>
 </sst>
 </file>
@@ -1065,13 +1068,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B51" sqref="B51"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,130 +1475,128 @@
       <c r="E22" s="4"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="8">
-        <v>42077</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="5">
+        <v>43356</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="5">
-        <v>42314</v>
+        <v>5</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="F24" s="8">
-        <v>42964</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42077</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D25" s="5">
-        <v>43017</v>
-      </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="8"/>
+        <v>42314</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="8">
+        <v>42964</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="5">
+        <v>43017</v>
+      </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>8</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D27" s="5"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="5">
-        <v>41914</v>
+        <v>8</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F28" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D29" s="5">
-        <v>42137</v>
+        <v>41914</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>60</v>
@@ -1604,25 +1605,33 @@
         <v>42137</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="5">
+        <v>42137</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F31" s="7">
         <v>42139</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1632,7 +1641,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1642,36 +1651,28 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F34" s="7">
-        <v>42138</v>
-      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="D35" s="5"/>
       <c r="E35" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F35" s="7">
-        <v>42137</v>
+        <v>42138</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1679,21 +1680,25 @@
         <v>12</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="3"/>
+      <c r="E36" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F36" s="7">
+        <v>42137</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="5" t="s">
@@ -1702,32 +1707,26 @@
       <c r="E37" s="4"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="5">
-        <v>41934</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="7">
-        <v>42138</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>47</v>
@@ -1747,57 +1746,57 @@
         <v>12</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="D40" s="5">
-        <v>42135</v>
+        <v>41934</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F40" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>38</v>
+        <v>61</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="5">
+        <v>42135</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F41" s="7">
         <v>42137</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D42" s="5">
+        <v>64</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="7">
         <v>42137</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F42" s="7">
-        <v>42138</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1805,7 +1804,7 @@
         <v>12</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>60</v>
@@ -1814,10 +1813,10 @@
         <v>42137</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F43" s="7">
-        <v>42137</v>
+        <v>42138</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1825,61 +1824,65 @@
         <v>12</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="D44" s="5">
-        <v>42176</v>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>42137</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="7">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="D45" s="5">
-        <v>42179</v>
+        <v>42176</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="7"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="D46" s="5">
-        <v>42242</v>
+        <v>42179</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="D47" s="5">
-        <v>42348</v>
+        <v>42242</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="7"/>
@@ -1889,47 +1892,43 @@
         <v>12</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D48" s="5">
-        <v>42619</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F48" s="7">
-        <v>43194</v>
-      </c>
+        <v>42348</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D49" s="5">
-        <v>42915</v>
+        <v>42619</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F49" s="5">
-        <v>42915</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="F49" s="7">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>60</v>
@@ -1937,48 +1936,54 @@
       <c r="D50" s="5">
         <v>42915</v>
       </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="5"/>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E50" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" s="5">
+        <v>42915</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="16" t="s">
-        <v>177</v>
+      <c r="B51" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D51" s="5">
-        <v>43228</v>
+        <v>42915</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="5">
+        <v>43228</v>
+      </c>
       <c r="E52" s="4"/>
-      <c r="F52" s="3"/>
+      <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C53" s="4"/>
-      <c r="D53" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="D53" s="5"/>
       <c r="E53" s="4"/>
       <c r="F53" s="3"/>
     </row>
@@ -1987,7 +1992,7 @@
         <v>15</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="5" t="s">
@@ -2001,81 +2006,79 @@
         <v>15</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E55" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F55" s="7">
-        <v>42138</v>
-      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D56" s="5">
+        <v>53</v>
+      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F56" s="7">
         <v>42138</v>
       </c>
-      <c r="E56" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F56" s="7">
-        <v>42139</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="D57" s="5">
-        <v>42137</v>
-      </c>
-      <c r="E57" s="4"/>
-      <c r="F57" s="3"/>
+        <v>42138</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F57" s="7">
+        <v>42139</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C58" s="4"/>
       <c r="D58" s="5">
-        <v>42138</v>
+        <v>42137</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D59" s="5">
-        <v>42348</v>
+        <v>42138</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="3"/>
@@ -2085,79 +2088,81 @@
         <v>15</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D60" s="5">
-        <v>43017</v>
+        <v>42348</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="3"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>90</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D61" s="5">
+        <v>43017</v>
+      </c>
+      <c r="E61" s="4"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F62" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F63" s="3"/>
+        <v>91</v>
+      </c>
+      <c r="F63" s="7">
+        <v>42146</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E64" s="4"/>
+      <c r="E64" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2165,261 +2170,259 @@
         <v>17</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="E65" s="4"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D66" s="5">
-        <v>42146</v>
-      </c>
-      <c r="E66" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D67" s="5">
-        <v>42163</v>
+        <v>42146</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D68" s="5">
-        <v>42066</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F68" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>42163</v>
+      </c>
+      <c r="E68" s="4"/>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D69" s="5">
-        <v>42023</v>
+        <v>42066</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F69" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="5" t="s">
-        <v>38</v>
+        <v>51</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" s="5">
+        <v>42023</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F70" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="F71" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="C72" s="4"/>
-      <c r="D72" s="5"/>
+      <c r="D72" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="E72" s="4" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="F72" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D73" s="5">
-        <v>42188</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C73" s="4"/>
+      <c r="D73" s="5"/>
       <c r="E73" s="4" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="F73" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>113</v>
+        <v>60</v>
       </c>
       <c r="D74" s="5">
-        <v>42193</v>
+        <v>42188</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>67</v>
       </c>
       <c r="F74" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="D75" s="5">
-        <v>42256</v>
+        <v>42193</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>67</v>
       </c>
       <c r="F75" s="7">
-        <v>42380</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D76" s="5">
-        <v>42472</v>
+        <v>42256</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="F76" s="7"/>
-    </row>
-    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="F76" s="7">
+        <v>42380</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B77" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77" s="5">
+        <v>42472</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F77" s="7"/>
+    </row>
+    <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D77" s="5">
+      <c r="C78" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D78" s="5">
         <v>43238</v>
       </c>
-      <c r="E77" s="4"/>
-      <c r="F77" s="7"/>
-    </row>
-    <row r="78" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C78" s="4"/>
-      <c r="D78" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="E78" s="4"/>
-      <c r="F78" s="3"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F78" s="7"/>
+    </row>
+    <row r="79" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D79" s="5">
-        <v>42157</v>
+        <v>124</v>
+      </c>
+      <c r="C79" s="4"/>
+      <c r="D79" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="3"/>
@@ -2429,75 +2432,71 @@
         <v>23</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="5" t="s">
-        <v>38</v>
+        <v>99</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D80" s="5">
+        <v>42157</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" s="4"/>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E82" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F81" s="7">
+      <c r="F82" s="7">
         <v>43194</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D82" s="5">
-        <v>42135</v>
-      </c>
-      <c r="E82" s="4"/>
-      <c r="F82" s="3"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="D83" s="5">
-        <v>42205</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F83" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>42135</v>
+      </c>
+      <c r="E83" s="4"/>
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>115</v>
@@ -2506,77 +2505,102 @@
         <v>42205</v>
       </c>
       <c r="E84" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F84" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D85" s="5">
+        <v>42205</v>
+      </c>
+      <c r="E85" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="F84" s="3" t="s">
+      <c r="F85" s="3" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F84"/>
-  <conditionalFormatting sqref="B73:B76 B68:B71 B3:B13 B15 B48:B50 B26:B46 B60:B66 B19:B24 B78:B82 B17 B52:B58">
-    <cfRule type="expression" dxfId="13" priority="19">
+  <autoFilter ref="A2:F85"/>
+  <conditionalFormatting sqref="B74:B77 B69:B72 B3:B13 B15 B49:B51 B27:B47 B61:B67 B19:B21 B79:B83 B17 B53:B59 B23:B25">
+    <cfRule type="expression" dxfId="14" priority="20">
       <formula>ISBLANK($F3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67">
-    <cfRule type="expression" dxfId="12" priority="14">
-      <formula>ISBLANK($F67)</formula>
+  <conditionalFormatting sqref="B68">
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>ISBLANK($F68)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B72">
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>ISBLANK($F72)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B83">
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>ISBLANK($F83)</formula>
+  <conditionalFormatting sqref="B73">
+    <cfRule type="expression" dxfId="12" priority="14">
+      <formula>ISBLANK($F73)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>ISBLANK($F84)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B85">
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>ISBLANK($F85)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>ISBLANK($F18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>ISBLANK($F14)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>ISBLANK($F47)</formula>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>ISBLANK($F48)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>ISBLANK($F25)</formula>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>ISBLANK($F26)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B59">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>ISBLANK($F59)</formula>
+  <conditionalFormatting sqref="B60">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>ISBLANK($F60)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B77">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>ISBLANK($F77)</formula>
+  <conditionalFormatting sqref="B78">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ISBLANK($F78)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>ISBLANK($F16)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51">
+  <conditionalFormatting sqref="B52">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>ISBLANK($F52)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>ISBLANK($F51)</formula>
+      <formula>ISBLANK($F22)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Added a new bug to fux 7mar2019
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="15000" windowHeight="6075"/>
+    <workbookView xWindow="120" yWindow="195" windowWidth="15000" windowHeight="6015"/>
   </bookViews>
   <sheets>
     <sheet name="To do" sheetId="1" r:id="rId1"/>
     <sheet name="versions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$F$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$87</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'To do'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="183">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -570,6 +570,12 @@
   </si>
   <si>
     <t>Michael Kundi</t>
+  </si>
+  <si>
+    <t>anova within compute_df seems to hang when I tried it with 2000 studies</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -698,17 +704,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1089,1560 +1085,1673 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B87" sqref="B87"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="56.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="6.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="7">
+      <c r="G3" s="7">
         <v>42135</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="7">
+      <c r="G4" s="7">
         <v>42135</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="5">
+      <c r="E6" s="5">
         <v>42045</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="7">
+      <c r="G6" s="7">
         <v>42076</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="5">
+      <c r="E7" s="5">
         <v>42157</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="7">
         <v>42163</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="5">
         <v>42166</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="5">
         <v>42166</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="5">
         <v>42191</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F10" s="7">
+      <c r="G10" s="7">
         <v>42191</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="5">
         <v>42191</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="7">
+      <c r="G11" s="7">
         <v>42191</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="5">
         <v>42242</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F12" s="4"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="5">
         <v>42256</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="5">
         <v>42314</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="F14" s="7">
+      <c r="G14" s="7">
         <v>43194</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="5">
+      <c r="E15" s="5">
         <v>42388</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F15" s="7">
+      <c r="G15" s="7">
         <v>43194</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="5">
         <v>43250</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="4"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D17" s="5">
+      <c r="E17" s="5">
         <v>43085</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="4"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="5">
-        <v>42045</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="5">
+        <v>43531</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>126</v>
-      </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="5">
+      <c r="E19" s="5">
         <v>42045</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="5">
+      <c r="E20" s="5">
         <v>42045</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="4"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="5">
+        <v>42045</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="7">
+      <c r="G21" s="7">
         <v>42135</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>122</v>
-      </c>
+      <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="5">
-        <v>42262</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>174</v>
-      </c>
+      <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="5">
-        <v>43238</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="5">
+        <v>42262</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="3"/>
+      <c r="C24" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="5">
+        <v>43238</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="5">
+      <c r="D25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="5">
         <v>43356</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="8">
-        <v>42077</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F25" s="4"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="B26" s="3"/>
       <c r="C26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="5">
-        <v>42314</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F26" s="8">
-        <v>42964</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="8">
+        <v>42077</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="5">
+        <v>42314</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="8">
+        <v>42964</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="5">
+      <c r="D28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="5">
         <v>43017</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="F28" s="4"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D29" s="4"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="B30" s="3"/>
       <c r="C30" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="5">
-        <v>41914</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="B31" s="3"/>
       <c r="C31" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="5">
-        <v>42137</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="5">
+        <v>41914</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3"/>
+      <c r="C32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="5">
+        <v>42137</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="5">
+      <c r="D33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="5">
         <v>42137</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="7">
+      <c r="G33" s="7">
         <v>42139</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D36" s="4"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="B37" s="3"/>
+      <c r="C37" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="7">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5" t="s">
+      <c r="B38" s="3"/>
+      <c r="C38" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G38" s="7">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5" t="s">
+      <c r="B39" s="3"/>
+      <c r="C39" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F39" s="4"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="B40" s="3"/>
       <c r="C40" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="5">
-        <v>41934</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F40" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="5">
+      <c r="E41" s="5">
         <v>41934</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="F41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F41" s="7">
+      <c r="G41" s="7">
         <v>42138</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5">
-        <v>42135</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F42" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+      <c r="C42" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="5">
+        <v>41934</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" s="7">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="B43" s="3"/>
       <c r="C43" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F43" s="7">
+        <v>61</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="5">
+        <v>42135</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G43" s="7">
         <v>42137</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="B44" s="3"/>
       <c r="C44" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" s="5">
+        <v>63</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G44" s="7">
         <v>42137</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F44" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="B45" s="3"/>
       <c r="C45" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="5">
+        <v>78</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="5">
         <v>42137</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F45" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F45" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G45" s="7">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>103</v>
-      </c>
+      <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" s="5">
-        <v>42176</v>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="7"/>
-    </row>
-    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="5">
+        <v>42137</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G46" s="7">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>105</v>
-      </c>
+      <c r="B47" s="3"/>
       <c r="C47" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" s="5">
-        <v>42179</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="7"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="5">
+        <v>42176</v>
+      </c>
+      <c r="F47" s="4"/>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D48" s="5">
-        <v>42242</v>
-      </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="7"/>
-    </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" s="5">
+        <v>42179</v>
+      </c>
+      <c r="F48" s="4"/>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>128</v>
-      </c>
+      <c r="B49" s="3"/>
       <c r="C49" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="5">
-        <v>42348</v>
-      </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="7"/>
-    </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="5">
+        <v>42242</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>134</v>
-      </c>
+      <c r="B50" s="3"/>
       <c r="C50" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="5">
-        <v>42619</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F50" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="5">
+        <v>42348</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="7"/>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="B51" s="3"/>
       <c r="C51" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" s="5">
-        <v>42915</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F51" s="5">
-        <v>42915</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" s="5">
+        <v>42619</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G51" s="7">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="B52" s="3"/>
       <c r="C52" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="5">
+        <v>135</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E52" s="5">
         <v>42915</v>
       </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="5"/>
-    </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F52" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G52" s="5">
+        <v>42915</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="3"/>
+      <c r="C53" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E53" s="5">
+        <v>42915</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D53" s="5">
+      <c r="D54" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E54" s="5">
         <v>43228</v>
       </c>
-      <c r="E53" s="4"/>
-      <c r="F53" s="5"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="4"/>
+      <c r="G54" s="5"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+      <c r="C55" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="3"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="5" t="s">
+      <c r="B56" s="3"/>
+      <c r="C56" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E56" s="4"/>
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="4"/>
+      <c r="G56" s="3"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="5" t="s">
+      <c r="B57" s="3"/>
+      <c r="C57" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F57" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="4"/>
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="B58" s="3"/>
       <c r="C58" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" s="5">
+        <v>53</v>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G58" s="7">
         <v>42138</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F58" s="7">
-        <v>42139</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="5">
-        <v>42137</v>
-      </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+      <c r="C59" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E59" s="5">
+        <v>42138</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G59" s="7">
+        <v>42139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="B60" s="3"/>
       <c r="C60" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D60" s="5">
-        <v>42138</v>
-      </c>
-      <c r="E60" s="4"/>
-      <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="5">
+        <v>42137</v>
+      </c>
+      <c r="F60" s="4"/>
+      <c r="G60" s="3"/>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>129</v>
-      </c>
+      <c r="B61" s="3"/>
       <c r="C61" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D61" s="5">
-        <v>42348</v>
-      </c>
-      <c r="E61" s="4"/>
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61" s="5">
+        <v>42138</v>
+      </c>
+      <c r="F61" s="4"/>
+      <c r="G61" s="3"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3"/>
+      <c r="C62" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" s="5">
+        <v>42348</v>
+      </c>
+      <c r="F62" s="4"/>
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D62" s="5">
+      <c r="D63" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E63" s="5">
         <v>43017</v>
       </c>
-      <c r="E62" s="4"/>
-      <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C63" s="4"/>
-      <c r="D63" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F63" s="4"/>
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B64" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="5" t="s">
+      <c r="B64" s="3"/>
+      <c r="C64" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E64" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F64" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="5" t="s">
+      <c r="B65" s="3"/>
+      <c r="C65" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="4"/>
+      <c r="E65" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G65" s="7">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="5" t="s">
+      <c r="B66" s="3"/>
+      <c r="C66" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="E66" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E66" s="4"/>
-      <c r="F66" s="3"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C67" s="4"/>
-      <c r="D67" s="5" t="s">
+      <c r="B67" s="3"/>
+      <c r="C67" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="4"/>
+      <c r="E67" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E67" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="F67" s="4"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>89</v>
-      </c>
+      <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D68" s="5">
-        <v>42146</v>
-      </c>
-      <c r="E68" s="4"/>
-      <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3"/>
+      <c r="C69" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E69" s="5">
+        <v>42146</v>
+      </c>
+      <c r="F69" s="4"/>
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D69" s="5">
+      <c r="D70" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E70" s="5">
         <v>42163</v>
       </c>
-      <c r="E69" s="4"/>
-      <c r="F69" s="3"/>
-    </row>
-    <row r="70" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D70" s="5">
-        <v>42066</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F70" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="F70" s="4"/>
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="B71" s="3"/>
       <c r="C71" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D71" s="5">
-        <v>42023</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F71" s="7">
+        <v>49</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E71" s="5">
+        <v>42066</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G71" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F72" s="7">
+      <c r="B72" s="3"/>
+      <c r="C72" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E72" s="5">
+        <v>42023</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G72" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="5" t="s">
+      <c r="B73" s="3"/>
+      <c r="C73" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" s="4"/>
+      <c r="E73" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E73" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F73" s="7">
+      <c r="F73" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G73" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B74" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F74" s="7">
+      <c r="B74" s="3"/>
+      <c r="C74" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D74" s="4"/>
+      <c r="E74" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G74" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B75" s="4" t="s">
-        <v>106</v>
-      </c>
+      <c r="B75" s="3"/>
       <c r="C75" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D75" s="5">
-        <v>42188</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F75" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="D75" s="4"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G75" s="7">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>112</v>
-      </c>
+      <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D76" s="5">
-        <v>42193</v>
-      </c>
-      <c r="E76" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E76" s="5">
+        <v>42188</v>
+      </c>
+      <c r="F76" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F76" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" s="7">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>119</v>
-      </c>
+      <c r="B77" s="3"/>
       <c r="C77" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D77" s="5">
-        <v>42256</v>
-      </c>
-      <c r="E77" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E77" s="5">
+        <v>42193</v>
+      </c>
+      <c r="F77" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F77" s="7">
-        <v>42380</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G77" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B78" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="B78" s="3"/>
       <c r="C78" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D78" s="5">
-        <v>42472</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="F78" s="7"/>
-    </row>
-    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E78" s="5">
+        <v>42256</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G78" s="7">
+        <v>42380</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3"/>
+      <c r="C79" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E79" s="5">
+        <v>42472</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G79" s="7"/>
+    </row>
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D79" s="5">
+      <c r="D80" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E80" s="5">
         <v>43238</v>
       </c>
-      <c r="E79" s="4"/>
-      <c r="F79" s="7"/>
-    </row>
-    <row r="80" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B80" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E80" s="4"/>
-      <c r="F80" s="3"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F80" s="4"/>
+      <c r="G80" s="7"/>
+    </row>
+    <row r="81" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D81" s="5">
-        <v>42157</v>
-      </c>
-      <c r="E81" s="4"/>
-      <c r="F81" s="3"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+      <c r="C81" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D81" s="4"/>
+      <c r="E81" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F81" s="4"/>
+      <c r="G81" s="3"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3"/>
+      <c r="C82" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E82" s="5">
+        <v>42157</v>
+      </c>
+      <c r="F82" s="4"/>
+      <c r="G82" s="3"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="3"/>
+      <c r="C83" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C82" s="4"/>
-      <c r="D82" s="5" t="s">
+      <c r="D83" s="4"/>
+      <c r="E83" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E82" s="4"/>
-      <c r="F82" s="3"/>
-    </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="F83" s="4"/>
+      <c r="G83" s="3"/>
+    </row>
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="3"/>
+      <c r="C84" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C83" s="4"/>
-      <c r="D83" s="5" t="s">
+      <c r="D84" s="4"/>
+      <c r="E84" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="F84" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F83" s="7">
+      <c r="G84" s="7">
         <v>43194</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D84" s="5">
-        <v>42135</v>
-      </c>
-      <c r="E84" s="4"/>
-      <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="B85" s="3"/>
       <c r="C85" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D85" s="5">
-        <v>42205</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F85" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E85" s="5">
+        <v>42135</v>
+      </c>
+      <c r="F85" s="4"/>
+      <c r="G85" s="3"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3"/>
+      <c r="C86" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E86" s="5">
+        <v>42205</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G86" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B87" s="3"/>
+      <c r="C87" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="D87" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D86" s="5">
+      <c r="E87" s="5">
         <v>42205</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="F87" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="F86" s="3" t="s">
+      <c r="G87" s="3" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F86"/>
-  <conditionalFormatting sqref="B75:B78 B70:B73 B3:B13 B15 B50:B52 B28:B48 B62:B68 B20:B22 B80:B84 B18 B54:B60 B24:B26">
-    <cfRule type="expression" dxfId="17" priority="22">
-      <formula>ISBLANK($F3)</formula>
+  <autoFilter ref="A2:G87"/>
+  <conditionalFormatting sqref="C76:C79 C71:C74 C3:C13 C15 C51:C53 C29:C49 C63:C69 C21:C23 C81:C85 C19 C55:C61 C25:C27">
+    <cfRule type="expression" dxfId="15" priority="23">
+      <formula>ISBLANK($G3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B69">
-    <cfRule type="expression" dxfId="16" priority="17">
-      <formula>ISBLANK($F69)</formula>
+  <conditionalFormatting sqref="C70">
+    <cfRule type="expression" dxfId="14" priority="18">
+      <formula>ISBLANK($G70)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B74">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>ISBLANK($F74)</formula>
+  <conditionalFormatting sqref="C75">
+    <cfRule type="expression" dxfId="13" priority="17">
+      <formula>ISBLANK($G75)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B85">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>ISBLANK($F85)</formula>
+  <conditionalFormatting sqref="C86">
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>ISBLANK($G86)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B86">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>ISBLANK($F86)</formula>
+  <conditionalFormatting sqref="C87">
+    <cfRule type="expression" dxfId="11" priority="15">
+      <formula>ISBLANK($G87)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="expression" dxfId="12" priority="13">
-      <formula>ISBLANK($F19)</formula>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>ISBLANK($G20)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="11" priority="12">
-      <formula>ISBLANK($F14)</formula>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="9" priority="13">
+      <formula>ISBLANK($G14)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
-    <cfRule type="expression" dxfId="10" priority="11">
-      <formula>ISBLANK($F49)</formula>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="expression" dxfId="8" priority="12">
+      <formula>ISBLANK($G50)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>ISBLANK($F27)</formula>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="expression" dxfId="7" priority="10">
+      <formula>ISBLANK($G28)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B61">
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>ISBLANK($F61)</formula>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>ISBLANK($G62)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B79">
-    <cfRule type="expression" dxfId="7" priority="6">
-      <formula>ISBLANK($F79)</formula>
+  <conditionalFormatting sqref="C80">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>ISBLANK($G80)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B53">
-    <cfRule type="expression" dxfId="5" priority="4">
-      <formula>ISBLANK($F53)</formula>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>ISBLANK($G54)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>ISBLANK($F23)</formula>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>ISBLANK($G24)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>ISBLANK($F16)</formula>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>ISBLANK($G16)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>ISBLANK($F17)</formula>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>ISBLANK($G18)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>ISBLANK($G17)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Added a new bug to be fixed 7mar2019
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="15000" windowHeight="6075"/>
+    <workbookView xWindow="120" yWindow="195" windowWidth="15000" windowHeight="6015"/>
   </bookViews>
   <sheets>
     <sheet name="To do" sheetId="1" r:id="rId1"/>
     <sheet name="versions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$F$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$87</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'To do'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="183">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -570,6 +570,12 @@
   </si>
   <si>
     <t>Michael Kundi</t>
+  </si>
+  <si>
+    <t>anova within compute_df seems to hang when I tried it with 2000 studies</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -698,17 +704,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1089,1560 +1085,1673 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B87" sqref="B87"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="56.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="6.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="7">
+      <c r="G3" s="7">
         <v>42135</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="7">
+      <c r="G4" s="7">
         <v>42135</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="5">
+      <c r="E6" s="5">
         <v>42045</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="7">
+      <c r="G6" s="7">
         <v>42076</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="5">
+      <c r="E7" s="5">
         <v>42157</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="7">
         <v>42163</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="5">
         <v>42166</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="5">
         <v>42166</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="5">
         <v>42191</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F10" s="7">
+      <c r="G10" s="7">
         <v>42191</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="5">
         <v>42191</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="7">
+      <c r="G11" s="7">
         <v>42191</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="5">
         <v>42242</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F12" s="4"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="5">
         <v>42256</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="5">
         <v>42314</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="F14" s="7">
+      <c r="G14" s="7">
         <v>43194</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="5">
+      <c r="E15" s="5">
         <v>42388</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F15" s="7">
+      <c r="G15" s="7">
         <v>43194</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="5">
         <v>43250</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="4"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D17" s="5">
+      <c r="E17" s="5">
         <v>43085</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="4"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="5">
-        <v>42045</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="5">
+        <v>43531</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>126</v>
-      </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="5">
+      <c r="E19" s="5">
         <v>42045</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="5">
+      <c r="E20" s="5">
         <v>42045</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="4"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="5">
+        <v>42045</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="7">
+      <c r="G21" s="7">
         <v>42135</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>122</v>
-      </c>
+      <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="5">
-        <v>42262</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>174</v>
-      </c>
+      <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="5">
-        <v>43238</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="5">
+        <v>42262</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="3"/>
+      <c r="C24" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="5">
+        <v>43238</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="5">
+      <c r="D25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="5">
         <v>43356</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="8">
-        <v>42077</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F25" s="4"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="B26" s="3"/>
       <c r="C26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="5">
-        <v>42314</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F26" s="8">
-        <v>42964</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="8">
+        <v>42077</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="5">
+        <v>42314</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="8">
+        <v>42964</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="5">
+      <c r="D28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="5">
         <v>43017</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="F28" s="4"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="D29" s="4"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="B30" s="3"/>
       <c r="C30" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="5">
-        <v>41914</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="B31" s="3"/>
       <c r="C31" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="5">
-        <v>42137</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="5">
+        <v>41914</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3"/>
+      <c r="C32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="5">
+        <v>42137</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="5">
+      <c r="D33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="5">
         <v>42137</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="7">
+      <c r="G33" s="7">
         <v>42139</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D36" s="4"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="B37" s="3"/>
+      <c r="C37" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="7">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5" t="s">
+      <c r="B38" s="3"/>
+      <c r="C38" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G38" s="7">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5" t="s">
+      <c r="B39" s="3"/>
+      <c r="C39" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F39" s="4"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="B40" s="3"/>
       <c r="C40" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="5">
-        <v>41934</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F40" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="5">
+      <c r="E41" s="5">
         <v>41934</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="F41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F41" s="7">
+      <c r="G41" s="7">
         <v>42138</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5">
-        <v>42135</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F42" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+      <c r="C42" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="5">
+        <v>41934</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" s="7">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="B43" s="3"/>
       <c r="C43" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F43" s="7">
+        <v>61</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="5">
+        <v>42135</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G43" s="7">
         <v>42137</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="B44" s="3"/>
       <c r="C44" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" s="5">
+        <v>63</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G44" s="7">
         <v>42137</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F44" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="B45" s="3"/>
       <c r="C45" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="5">
+        <v>78</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="5">
         <v>42137</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F45" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F45" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G45" s="7">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>103</v>
-      </c>
+      <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" s="5">
-        <v>42176</v>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="7"/>
-    </row>
-    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="5">
+        <v>42137</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G46" s="7">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>105</v>
-      </c>
+      <c r="B47" s="3"/>
       <c r="C47" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" s="5">
-        <v>42179</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="7"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="5">
+        <v>42176</v>
+      </c>
+      <c r="F47" s="4"/>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D48" s="5">
-        <v>42242</v>
-      </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="7"/>
-    </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" s="5">
+        <v>42179</v>
+      </c>
+      <c r="F48" s="4"/>
+      <c r="G48" s="7"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>128</v>
-      </c>
+      <c r="B49" s="3"/>
       <c r="C49" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="5">
-        <v>42348</v>
-      </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="7"/>
-    </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="5">
+        <v>42242</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>134</v>
-      </c>
+      <c r="B50" s="3"/>
       <c r="C50" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="5">
-        <v>42619</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F50" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="5">
+        <v>42348</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="7"/>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="B51" s="3"/>
       <c r="C51" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" s="5">
-        <v>42915</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F51" s="5">
-        <v>42915</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" s="5">
+        <v>42619</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G51" s="7">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="B52" s="3"/>
       <c r="C52" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="5">
+        <v>135</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E52" s="5">
         <v>42915</v>
       </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="5"/>
-    </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F52" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G52" s="5">
+        <v>42915</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="3"/>
+      <c r="C53" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E53" s="5">
+        <v>42915</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D53" s="5">
+      <c r="D54" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E54" s="5">
         <v>43228</v>
       </c>
-      <c r="E53" s="4"/>
-      <c r="F53" s="5"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="4"/>
+      <c r="G54" s="5"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E55" s="4"/>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+      <c r="C55" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="3"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="5" t="s">
+      <c r="B56" s="3"/>
+      <c r="C56" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E56" s="4"/>
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="4"/>
+      <c r="G56" s="3"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="5" t="s">
+      <c r="B57" s="3"/>
+      <c r="C57" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F57" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="4"/>
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="B58" s="3"/>
       <c r="C58" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" s="5">
+        <v>53</v>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G58" s="7">
         <v>42138</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F58" s="7">
-        <v>42139</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="5">
-        <v>42137</v>
-      </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+      <c r="C59" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E59" s="5">
+        <v>42138</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G59" s="7">
+        <v>42139</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="B60" s="3"/>
       <c r="C60" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D60" s="5">
-        <v>42138</v>
-      </c>
-      <c r="E60" s="4"/>
-      <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="5">
+        <v>42137</v>
+      </c>
+      <c r="F60" s="4"/>
+      <c r="G60" s="3"/>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>129</v>
-      </c>
+      <c r="B61" s="3"/>
       <c r="C61" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D61" s="5">
-        <v>42348</v>
-      </c>
-      <c r="E61" s="4"/>
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61" s="5">
+        <v>42138</v>
+      </c>
+      <c r="F61" s="4"/>
+      <c r="G61" s="3"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3"/>
+      <c r="C62" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" s="5">
+        <v>42348</v>
+      </c>
+      <c r="F62" s="4"/>
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D62" s="5">
+      <c r="D63" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E63" s="5">
         <v>43017</v>
       </c>
-      <c r="E62" s="4"/>
-      <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C63" s="4"/>
-      <c r="D63" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F63" s="4"/>
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B64" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="5" t="s">
+      <c r="B64" s="3"/>
+      <c r="C64" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E64" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F64" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="5" t="s">
+      <c r="B65" s="3"/>
+      <c r="C65" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="4"/>
+      <c r="E65" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G65" s="7">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B66" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="5" t="s">
+      <c r="B66" s="3"/>
+      <c r="C66" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="E66" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E66" s="4"/>
-      <c r="F66" s="3"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C67" s="4"/>
-      <c r="D67" s="5" t="s">
+      <c r="B67" s="3"/>
+      <c r="C67" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="4"/>
+      <c r="E67" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E67" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="F67" s="4"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>89</v>
-      </c>
+      <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D68" s="5">
-        <v>42146</v>
-      </c>
-      <c r="E68" s="4"/>
-      <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3"/>
+      <c r="C69" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E69" s="5">
+        <v>42146</v>
+      </c>
+      <c r="F69" s="4"/>
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D69" s="5">
+      <c r="D70" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E70" s="5">
         <v>42163</v>
       </c>
-      <c r="E69" s="4"/>
-      <c r="F69" s="3"/>
-    </row>
-    <row r="70" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D70" s="5">
-        <v>42066</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F70" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="F70" s="4"/>
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="B71" s="3"/>
       <c r="C71" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D71" s="5">
-        <v>42023</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F71" s="7">
+        <v>49</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E71" s="5">
+        <v>42066</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G71" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F72" s="7">
+      <c r="B72" s="3"/>
+      <c r="C72" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E72" s="5">
+        <v>42023</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G72" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="5" t="s">
+      <c r="B73" s="3"/>
+      <c r="C73" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D73" s="4"/>
+      <c r="E73" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E73" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F73" s="7">
+      <c r="F73" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G73" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B74" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F74" s="7">
+      <c r="B74" s="3"/>
+      <c r="C74" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D74" s="4"/>
+      <c r="E74" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G74" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B75" s="4" t="s">
-        <v>106</v>
-      </c>
+      <c r="B75" s="3"/>
       <c r="C75" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D75" s="5">
-        <v>42188</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F75" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="D75" s="4"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G75" s="7">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>112</v>
-      </c>
+      <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D76" s="5">
-        <v>42193</v>
-      </c>
-      <c r="E76" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E76" s="5">
+        <v>42188</v>
+      </c>
+      <c r="F76" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F76" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" s="7">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>119</v>
-      </c>
+      <c r="B77" s="3"/>
       <c r="C77" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D77" s="5">
-        <v>42256</v>
-      </c>
-      <c r="E77" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E77" s="5">
+        <v>42193</v>
+      </c>
+      <c r="F77" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F77" s="7">
-        <v>42380</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G77" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B78" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="B78" s="3"/>
       <c r="C78" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D78" s="5">
-        <v>42472</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="F78" s="7"/>
-    </row>
-    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E78" s="5">
+        <v>42256</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G78" s="7">
+        <v>42380</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3"/>
+      <c r="C79" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E79" s="5">
+        <v>42472</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G79" s="7"/>
+    </row>
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D79" s="5">
+      <c r="D80" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E80" s="5">
         <v>43238</v>
       </c>
-      <c r="E79" s="4"/>
-      <c r="F79" s="7"/>
-    </row>
-    <row r="80" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B80" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E80" s="4"/>
-      <c r="F80" s="3"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F80" s="4"/>
+      <c r="G80" s="7"/>
+    </row>
+    <row r="81" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D81" s="5">
-        <v>42157</v>
-      </c>
-      <c r="E81" s="4"/>
-      <c r="F81" s="3"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+      <c r="C81" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D81" s="4"/>
+      <c r="E81" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F81" s="4"/>
+      <c r="G81" s="3"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3"/>
+      <c r="C82" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E82" s="5">
+        <v>42157</v>
+      </c>
+      <c r="F82" s="4"/>
+      <c r="G82" s="3"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="3"/>
+      <c r="C83" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C82" s="4"/>
-      <c r="D82" s="5" t="s">
+      <c r="D83" s="4"/>
+      <c r="E83" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E82" s="4"/>
-      <c r="F82" s="3"/>
-    </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="F83" s="4"/>
+      <c r="G83" s="3"/>
+    </row>
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="3"/>
+      <c r="C84" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C83" s="4"/>
-      <c r="D83" s="5" t="s">
+      <c r="D84" s="4"/>
+      <c r="E84" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="F84" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F83" s="7">
+      <c r="G84" s="7">
         <v>43194</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D84" s="5">
-        <v>42135</v>
-      </c>
-      <c r="E84" s="4"/>
-      <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="B85" s="3"/>
       <c r="C85" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D85" s="5">
-        <v>42205</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F85" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E85" s="5">
+        <v>42135</v>
+      </c>
+      <c r="F85" s="4"/>
+      <c r="G85" s="3"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3"/>
+      <c r="C86" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E86" s="5">
+        <v>42205</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G86" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B87" s="3"/>
+      <c r="C87" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="D87" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D86" s="5">
+      <c r="E87" s="5">
         <v>42205</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="F87" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="F86" s="3" t="s">
+      <c r="G87" s="3" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F86"/>
-  <conditionalFormatting sqref="B75:B78 B70:B73 B3:B13 B15 B50:B52 B28:B48 B62:B68 B20:B22 B80:B84 B18 B54:B60 B24:B26">
-    <cfRule type="expression" dxfId="17" priority="22">
-      <formula>ISBLANK($F3)</formula>
+  <autoFilter ref="A2:G87"/>
+  <conditionalFormatting sqref="C76:C79 C71:C74 C3:C13 C15 C51:C53 C29:C49 C63:C69 C21:C23 C81:C85 C19 C55:C61 C25:C27">
+    <cfRule type="expression" dxfId="15" priority="23">
+      <formula>ISBLANK($G3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B69">
-    <cfRule type="expression" dxfId="16" priority="17">
-      <formula>ISBLANK($F69)</formula>
+  <conditionalFormatting sqref="C70">
+    <cfRule type="expression" dxfId="14" priority="18">
+      <formula>ISBLANK($G70)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B74">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>ISBLANK($F74)</formula>
+  <conditionalFormatting sqref="C75">
+    <cfRule type="expression" dxfId="13" priority="17">
+      <formula>ISBLANK($G75)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B85">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>ISBLANK($F85)</formula>
+  <conditionalFormatting sqref="C86">
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>ISBLANK($G86)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B86">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>ISBLANK($F86)</formula>
+  <conditionalFormatting sqref="C87">
+    <cfRule type="expression" dxfId="11" priority="15">
+      <formula>ISBLANK($G87)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="expression" dxfId="12" priority="13">
-      <formula>ISBLANK($F19)</formula>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>ISBLANK($G20)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="11" priority="12">
-      <formula>ISBLANK($F14)</formula>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="9" priority="13">
+      <formula>ISBLANK($G14)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
-    <cfRule type="expression" dxfId="10" priority="11">
-      <formula>ISBLANK($F49)</formula>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="expression" dxfId="8" priority="12">
+      <formula>ISBLANK($G50)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>ISBLANK($F27)</formula>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="expression" dxfId="7" priority="10">
+      <formula>ISBLANK($G28)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B61">
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>ISBLANK($F61)</formula>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>ISBLANK($G62)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B79">
-    <cfRule type="expression" dxfId="7" priority="6">
-      <formula>ISBLANK($F79)</formula>
+  <conditionalFormatting sqref="C80">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>ISBLANK($G80)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B53">
-    <cfRule type="expression" dxfId="5" priority="4">
-      <formula>ISBLANK($F53)</formula>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>ISBLANK($G54)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>ISBLANK($F23)</formula>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>ISBLANK($G24)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>ISBLANK($F16)</formula>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>ISBLANK($G16)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>ISBLANK($F17)</formula>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>ISBLANK($G18)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>ISBLANK($G17)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Known bug - nested treatment labels with network import
Added to spreadsheet and help file.
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -11,7 +11,7 @@
     <sheet name="versions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$90</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'To do'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="187">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -576,6 +576,18 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Failes from pairs format with nested treatment names</t>
+  </si>
+  <si>
+    <t>Ewelina</t>
+  </si>
+  <si>
+    <t>fails when study names include hyphens [error not seen]</t>
+  </si>
+  <si>
+    <t>labels can fail if imported as pairs [error not seen]</t>
   </si>
 </sst>
 </file>
@@ -658,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -700,11 +712,56 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1085,13 +1142,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,24 +1500,20 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="5">
-        <v>42045</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="7">
-        <v>42135</v>
-      </c>
+      <c r="C19" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="E19" s="19">
+        <v>43593</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1468,7 +1521,7 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>43</v>
@@ -1476,16 +1529,20 @@
       <c r="E20" s="5">
         <v>42045</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="4" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>43</v>
@@ -1493,24 +1550,22 @@
       <c r="E21" s="5">
         <v>42045</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="4"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5" t="s">
-        <v>38</v>
+        <v>65</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="5">
+        <v>42045</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>66</v>
@@ -1519,22 +1574,24 @@
         <v>42135</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E23" s="5">
-        <v>42262</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="7">
+        <v>42135</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -1542,13 +1599,13 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="4" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="E24" s="5">
-        <v>43238</v>
+        <v>42262</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="7"/>
@@ -1558,142 +1615,138 @@
         <v>2</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="16" t="s">
-        <v>178</v>
+      <c r="C25" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E25" s="5">
-        <v>43356</v>
+        <v>43238</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G26" s="8">
-        <v>42077</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="5">
-        <v>42314</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G27" s="8">
-        <v>42964</v>
-      </c>
+      <c r="C26" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="5">
+        <v>43356</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="E27" s="19">
+        <v>43593</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="5">
-        <v>43017</v>
-      </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="8">
+        <v>42077</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="3"/>
+      <c r="C29" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="5">
+        <v>42314</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G29" s="8">
+        <v>42964</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G30" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="5">
+        <v>43017</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="5">
-        <v>41914</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="4"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="5">
-        <v>42137</v>
+        <v>8</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G32" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="G32" s="7">
+        <v>42135</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
@@ -1701,102 +1754,106 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="5">
+        <v>41914</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="5">
+        <v>42137</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="5">
+      <c r="D35" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="5">
         <v>42137</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F35" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G35" s="7">
         <v>42139</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="3"/>
+      <c r="C36" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="E36" s="19">
+        <v>43593</v>
+      </c>
+      <c r="F36" s="18"/>
+      <c r="G36" s="20"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B37" s="3"/>
-      <c r="C37" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G37" s="7">
-        <v>42138</v>
-      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B38" s="3"/>
-      <c r="C38" s="4" t="s">
-        <v>81</v>
-      </c>
+      <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G38" s="7">
-        <v>42137</v>
-      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B39" s="3"/>
-      <c r="C39" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="E39" s="5"/>
       <c r="F39" s="4"/>
       <c r="G39" s="3"/>
     </row>
@@ -1806,95 +1863,85 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="4" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="D40" s="4"/>
-      <c r="E40" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F40" s="4"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E40" s="5"/>
+      <c r="F40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G40" s="7">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E41" s="5">
-        <v>41934</v>
+        <v>81</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G41" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E42" s="5">
-        <v>41934</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G42" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" s="4"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="4" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="D43" s="4"/>
-      <c r="E43" s="5">
-        <v>42135</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G43" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E43" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="4" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
+      </c>
+      <c r="E44" s="5">
+        <v>41934</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G44" s="7">
-        <v>42137</v>
+        <v>42138</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1903,16 +1950,16 @@
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="4" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E45" s="5">
-        <v>42137</v>
+        <v>41934</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G45" s="7">
         <v>42138</v>
@@ -1924,71 +1971,81 @@
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D46" s="4"/>
       <c r="E46" s="5">
-        <v>42137</v>
+        <v>42135</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G46" s="7">
         <v>42137</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="4" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E47" s="5">
-        <v>42176</v>
-      </c>
-      <c r="F47" s="4"/>
-      <c r="G47" s="7"/>
-    </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G47" s="7">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E48" s="5">
-        <v>42179</v>
-      </c>
-      <c r="F48" s="4"/>
-      <c r="G48" s="7"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42137</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G48" s="7">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="4" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="E49" s="5">
-        <v>42242</v>
-      </c>
-      <c r="F49" s="4"/>
-      <c r="G49" s="7"/>
+        <v>42137</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G49" s="7">
+        <v>42137</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
@@ -1996,135 +2053,143 @@
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="4" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="E50" s="5">
-        <v>42348</v>
+        <v>42176</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="7"/>
     </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="4" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E51" s="5">
-        <v>42619</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="G51" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42179</v>
+      </c>
+      <c r="F51" s="4"/>
+      <c r="G51" s="7"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="4" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="E52" s="5">
-        <v>42915</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G52" s="5">
-        <v>42915</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>42242</v>
+      </c>
+      <c r="F52" s="4"/>
+      <c r="G52" s="7"/>
+    </row>
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="4" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E53" s="5">
-        <v>42915</v>
+        <v>42348</v>
       </c>
       <c r="F53" s="4"/>
-      <c r="G53" s="5"/>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B54" s="3"/>
-      <c r="C54" s="16" t="s">
-        <v>177</v>
+      <c r="C54" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E54" s="5">
-        <v>43228</v>
-      </c>
-      <c r="F54" s="4"/>
-      <c r="G54" s="5"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42619</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G54" s="7">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="3"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" s="5">
+        <v>42915</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G55" s="5">
+        <v>42915</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="5" t="s">
-        <v>38</v>
+        <v>137</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E56" s="5">
+        <v>42915</v>
       </c>
       <c r="F56" s="4"/>
-      <c r="G56" s="3"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B57" s="3"/>
-      <c r="C57" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D57" s="4"/>
-      <c r="E57" s="5" t="s">
-        <v>38</v>
+      <c r="C57" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E57" s="5">
+        <v>43228</v>
       </c>
       <c r="F57" s="4"/>
-      <c r="G57" s="3"/>
+      <c r="G57" s="5"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
@@ -2132,18 +2197,12 @@
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="4" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D58" s="4"/>
-      <c r="E58" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G58" s="7">
-        <v>42138</v>
-      </c>
+      <c r="E58" s="5"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
@@ -2151,52 +2210,48 @@
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E59" s="5">
-        <v>42138</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G59" s="7">
-        <v>42139</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59" s="4"/>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="4" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="D60" s="4"/>
-      <c r="E60" s="5">
-        <v>42137</v>
+      <c r="E60" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E61" s="5">
+        <v>53</v>
+      </c>
+      <c r="D61" s="4"/>
+      <c r="E61" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G61" s="7">
         <v>42138</v>
       </c>
-      <c r="F61" s="4"/>
-      <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
@@ -2204,85 +2259,85 @@
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="4" t="s">
-        <v>129</v>
+        <v>84</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E62" s="5">
-        <v>42348</v>
-      </c>
-      <c r="F62" s="4"/>
-      <c r="G62" s="3"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42138</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G62" s="7">
+        <v>42139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D63" s="4"/>
       <c r="E63" s="5">
-        <v>43017</v>
+        <v>42137</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64" s="4"/>
-      <c r="E64" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>90</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E64" s="5">
+        <v>42138</v>
+      </c>
+      <c r="F64" s="4"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D65" s="4"/>
-      <c r="E65" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G65" s="7">
-        <v>42146</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E65" s="5">
+        <v>42348</v>
+      </c>
+      <c r="F65" s="4"/>
+      <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D66" s="4"/>
-      <c r="E66" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>92</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E66" s="5">
+        <v>43017</v>
+      </c>
+      <c r="F66" s="4"/>
       <c r="G66" s="3"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2291,244 +2346,236 @@
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F67" s="4"/>
+      <c r="F67" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G68" s="3"/>
-    </row>
-    <row r="69" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="G68" s="7">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E69" s="5">
-        <v>42146</v>
-      </c>
-      <c r="F69" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="D69" s="4"/>
+      <c r="E69" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="G69" s="3"/>
     </row>
-    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E70" s="5">
-        <v>42163</v>
+        <v>20</v>
+      </c>
+      <c r="D70" s="4"/>
+      <c r="E70" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="3"/>
     </row>
-    <row r="71" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E71" s="5">
-        <v>42066</v>
+        <v>21</v>
+      </c>
+      <c r="D71" s="4"/>
+      <c r="E71" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G71" s="7">
-        <v>42146</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="4" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E72" s="5">
-        <v>42023</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G72" s="7">
         <v>42146</v>
       </c>
+      <c r="F72" s="4"/>
+      <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D73" s="4"/>
-      <c r="E73" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G73" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E73" s="5">
+        <v>42163</v>
+      </c>
+      <c r="F73" s="4"/>
+      <c r="G73" s="3"/>
+    </row>
+    <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D74" s="4"/>
-      <c r="E74" s="5" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E74" s="5">
+        <v>42066</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="G74" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D75" s="4"/>
-      <c r="E75" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E75" s="5">
+        <v>42023</v>
+      </c>
       <c r="F75" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G75" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E76" s="5">
-        <v>42188</v>
+        <v>82</v>
+      </c>
+      <c r="D76" s="4"/>
+      <c r="E76" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="G76" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E77" s="5">
-        <v>42193</v>
+        <v>32</v>
+      </c>
+      <c r="D77" s="4"/>
+      <c r="E77" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F77" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G77" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E78" s="5">
-        <v>42256</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D78" s="4"/>
+      <c r="E78" s="5"/>
       <c r="F78" s="4" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="G78" s="7">
-        <v>42380</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="4" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E79" s="5">
-        <v>42472</v>
+        <v>42188</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G79" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="G79" s="7">
+        <v>43194</v>
+      </c>
     </row>
     <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
@@ -2536,222 +2583,298 @@
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="4" t="s">
-        <v>175</v>
+        <v>112</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="E80" s="5">
-        <v>43238</v>
-      </c>
-      <c r="F80" s="4"/>
-      <c r="G80" s="7"/>
-    </row>
-    <row r="81" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>42193</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G80" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B81" s="3"/>
-      <c r="C81" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D81" s="4"/>
-      <c r="E81" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F81" s="4"/>
-      <c r="G81" s="3"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C81" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E81" s="5">
+        <v>42256</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G81" s="7">
+        <v>42380</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="4" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E82" s="5">
-        <v>42157</v>
-      </c>
-      <c r="F82" s="4"/>
-      <c r="G82" s="3"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42472</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G82" s="7"/>
+    </row>
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D83" s="4"/>
-      <c r="E83" s="5" t="s">
-        <v>38</v>
+        <v>175</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E83" s="5">
+        <v>43238</v>
       </c>
       <c r="F83" s="4"/>
-      <c r="G83" s="3"/>
-    </row>
-    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G83" s="7"/>
+    </row>
+    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B84" s="3"/>
-      <c r="C84" s="4" t="s">
-        <v>26</v>
+      <c r="C84" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F84" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G84" s="7">
-        <v>43194</v>
-      </c>
+      <c r="F84" s="4"/>
+      <c r="G84" s="3"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="4" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E85" s="5">
-        <v>42135</v>
+        <v>42157</v>
       </c>
       <c r="F85" s="4"/>
       <c r="G85" s="3"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E86" s="5">
-        <v>42205</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G86" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="D86" s="4"/>
+      <c r="E86" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F86" s="4"/>
+      <c r="G86" s="3"/>
+    </row>
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D87" s="4"/>
+      <c r="E87" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G87" s="7">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="C88" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E88" s="5">
+        <v>42135</v>
+      </c>
+      <c r="F88" s="4"/>
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B89" s="3"/>
+      <c r="C89" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E89" s="5">
+        <v>42205</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G89" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="C90" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D90" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E87" s="5">
+      <c r="E90" s="5">
         <v>42205</v>
       </c>
-      <c r="F87" s="4" t="s">
+      <c r="F90" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="G87" s="3" t="s">
+      <c r="G90" s="3" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G87"/>
-  <conditionalFormatting sqref="C76:C79 C71:C74 C3:C13 C15 C51:C53 C29:C49 C63:C69 C21:C23 C81:C85 C19 C55:C61 C25:C27">
-    <cfRule type="expression" dxfId="15" priority="23">
+  <autoFilter ref="A2:G90"/>
+  <conditionalFormatting sqref="C79:C82 C74:C77 C3:C13 C15 C54:C56 C31:C35 C66:C72 C22:C24 C84:C88 C20 C58:C64 C26 C28:C29 C37:C52">
+    <cfRule type="expression" dxfId="19" priority="26">
       <formula>ISBLANK($G3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C70">
-    <cfRule type="expression" dxfId="14" priority="18">
-      <formula>ISBLANK($G70)</formula>
+  <conditionalFormatting sqref="C73">
+    <cfRule type="expression" dxfId="18" priority="21">
+      <formula>ISBLANK($G73)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C75">
-    <cfRule type="expression" dxfId="13" priority="17">
-      <formula>ISBLANK($G75)</formula>
+  <conditionalFormatting sqref="C78">
+    <cfRule type="expression" dxfId="17" priority="20">
+      <formula>ISBLANK($G78)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C86">
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>ISBLANK($G86)</formula>
+  <conditionalFormatting sqref="C89">
+    <cfRule type="expression" dxfId="16" priority="19">
+      <formula>ISBLANK($G89)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C87">
-    <cfRule type="expression" dxfId="11" priority="15">
-      <formula>ISBLANK($G87)</formula>
+  <conditionalFormatting sqref="C90">
+    <cfRule type="expression" dxfId="15" priority="18">
+      <formula>ISBLANK($G90)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="10" priority="14">
-      <formula>ISBLANK($G20)</formula>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="expression" dxfId="14" priority="17">
+      <formula>ISBLANK($G21)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="9" priority="13">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>ISBLANK($G14)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="8" priority="12">
-      <formula>ISBLANK($G50)</formula>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="expression" dxfId="12" priority="15">
+      <formula>ISBLANK($G53)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="7" priority="10">
-      <formula>ISBLANK($G28)</formula>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>ISBLANK($G30)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="6" priority="9">
-      <formula>ISBLANK($G62)</formula>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>ISBLANK($G65)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C80">
-    <cfRule type="expression" dxfId="5" priority="7">
-      <formula>ISBLANK($G80)</formula>
+  <conditionalFormatting sqref="C83">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>ISBLANK($G83)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>ISBLANK($G54)</formula>
+  <conditionalFormatting sqref="C57">
+    <cfRule type="expression" dxfId="8" priority="8">
+      <formula>ISBLANK($G57)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>ISBLANK($G24)</formula>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>ISBLANK($G25)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>ISBLANK($G16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>ISBLANK($G18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>ISBLANK($G17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>ISBLANK($G27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>ISBLANK($G19)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>ISBLANK($G36)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Fix network map problem.
It now detects version of networkplot and labels treatments accordingly. 
Also improve network table.
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Old Home Drives\ado\ian\network\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="195" windowWidth="15000" windowHeight="6015"/>
   </bookViews>
@@ -11,15 +16,44 @@
     <sheet name="versions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$91</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'To do'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ian White</author>
+  </authors>
+  <commentList>
+    <comment ref="C20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">use http://www.homepages.ucl.ac.uk/~rmjwiww/stata/meta/thromb.dta, clear
+encode treat, gen(trt)
+drop treat
+label def trt 1 "SK" 2 "AtPA" 3 "tPA" 6 "Ret"  5 "Ten"  4 "SK+tPA"  7 "UK"  8 "ASPAC", modify
+network setup r n, studyvar(study) trtvar(trt) nocodes
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="189">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -589,12 +623,18 @@
   <si>
     <t>labels can fail if imported as pairs [error not seen]</t>
   </si>
+  <si>
+    <t>nocodes option fails with confusing error message when treatment names contain "+"</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,6 +667,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -731,17 +778,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -848,6 +885,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -895,7 +935,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -930,7 +970,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1138,17 +1178,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,26 +1555,22 @@
       <c r="F19" s="4"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="5">
-        <v>42045</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="7">
-        <v>42135</v>
-      </c>
+      <c r="C20" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="19">
+        <v>43712</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1542,7 +1578,7 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>43</v>
@@ -1550,16 +1586,20 @@
       <c r="E21" s="5">
         <v>42045</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>43</v>
@@ -1567,24 +1607,22 @@
       <c r="E22" s="5">
         <v>42045</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F22" s="4"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5" t="s">
-        <v>38</v>
+        <v>65</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="5">
+        <v>42045</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>66</v>
@@ -1593,22 +1631,24 @@
         <v>42135</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E24" s="5">
-        <v>42262</v>
-      </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="7">
+        <v>42135</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -1616,13 +1656,13 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="4" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="E25" s="5">
-        <v>43238</v>
+        <v>42262</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="7"/>
@@ -1632,167 +1672,169 @@
         <v>2</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="16" t="s">
-        <v>178</v>
+      <c r="C26" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E26" s="5">
-        <v>43356</v>
+        <v>43238</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="5">
+        <v>43356</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D28" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E28" s="19">
         <v>43593</v>
       </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28" s="8">
-        <v>42077</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F28" s="18"/>
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="5">
-        <v>42314</v>
+        <v>5</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="G29" s="8">
-        <v>42964</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42077</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="16" t="s">
-        <v>149</v>
+      <c r="C30" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E30" s="5">
-        <v>43017</v>
-      </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="8"/>
+        <v>42314</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G30" s="8">
+        <v>42964</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="3"/>
+      <c r="C31" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="5">
+        <v>43017</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G31" s="8">
+        <v>43712</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G32" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E32" s="5"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="5">
-        <v>41914</v>
+        <v>8</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="G33" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="4" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E34" s="5">
-        <v>42137</v>
+        <v>41914</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>60</v>
@@ -1801,43 +1843,51 @@
         <v>42137</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="7">
-        <v>42139</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="E36" s="19">
-        <v>43593</v>
-      </c>
-      <c r="F36" s="18"/>
-      <c r="G36" s="20"/>
+        <v>75</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="5">
+        <v>42137</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G36" s="7">
+        <v>42139</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="3"/>
+      <c r="C37" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="E37" s="19">
+        <v>43593</v>
+      </c>
+      <c r="F37" s="18"/>
+      <c r="G37" s="20"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
@@ -1848,7 +1898,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
@@ -1859,20 +1909,14 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
-      <c r="F40" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G40" s="7">
-        <v>42138</v>
-      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -1880,17 +1924,15 @@
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="E41" s="5"/>
       <c r="F41" s="4" t="s">
         <v>73</v>
       </c>
       <c r="G41" s="7">
-        <v>42137</v>
+        <v>42138</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1899,14 +1941,18 @@
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="4" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="3"/>
+      <c r="F42" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G42" s="7">
+        <v>42137</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -1914,7 +1960,7 @@
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="5" t="s">
@@ -1923,26 +1969,20 @@
       <c r="F43" s="4"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E44" s="5">
-        <v>41934</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G44" s="7">
-        <v>42138</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="4"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
@@ -1950,7 +1990,7 @@
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>47</v>
@@ -1971,59 +2011,59 @@
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="E46" s="5">
-        <v>42135</v>
+        <v>41934</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G46" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>38</v>
+        <v>61</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="5">
+        <v>42135</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G47" s="7">
         <v>42137</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E48" s="5">
+        <v>64</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G48" s="7">
         <v>42137</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G48" s="7">
-        <v>42138</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2032,7 +2072,7 @@
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>60</v>
@@ -2041,10 +2081,10 @@
         <v>42137</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G49" s="7">
-        <v>42137</v>
+        <v>42138</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2053,64 +2093,68 @@
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="4" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="E50" s="5">
-        <v>42176</v>
-      </c>
-      <c r="F50" s="4"/>
-      <c r="G50" s="7"/>
-    </row>
-    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>42137</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G50" s="7">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="E51" s="5">
-        <v>42179</v>
+        <v>42176</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="4" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="E52" s="5">
-        <v>42242</v>
+        <v>42179</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="4" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="E53" s="5">
-        <v>42348</v>
+        <v>42242</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="7"/>
@@ -2121,20 +2165,16 @@
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E54" s="5">
-        <v>42619</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="G54" s="7">
-        <v>43194</v>
-      </c>
+        <v>42348</v>
+      </c>
+      <c r="F54" s="4"/>
+      <c r="G54" s="7"/>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
@@ -2142,28 +2182,28 @@
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E55" s="5">
-        <v>42915</v>
+        <v>42619</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G55" s="5">
-        <v>42915</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="G55" s="7">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>60</v>
@@ -2171,38 +2211,46 @@
       <c r="E56" s="5">
         <v>42915</v>
       </c>
-      <c r="F56" s="4"/>
-      <c r="G56" s="5"/>
-    </row>
-    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F56" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G56" s="5">
+        <v>42915</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B57" s="3"/>
-      <c r="C57" s="16" t="s">
-        <v>177</v>
+      <c r="C57" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E57" s="5">
-        <v>43228</v>
+        <v>42915</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="5"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B58" s="3"/>
-      <c r="C58" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D58" s="4"/>
-      <c r="E58" s="5"/>
+      <c r="C58" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58" s="5">
+        <v>43228</v>
+      </c>
       <c r="F58" s="4"/>
-      <c r="G58" s="3"/>
+      <c r="G58" s="5"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
@@ -2210,12 +2258,10 @@
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D59" s="4"/>
-      <c r="E59" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="E59" s="5"/>
       <c r="F59" s="4"/>
       <c r="G59" s="3"/>
     </row>
@@ -2225,7 +2271,7 @@
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="5" t="s">
@@ -2240,18 +2286,14 @@
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="4" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F61" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G61" s="7">
-        <v>42138</v>
-      </c>
+      <c r="F61" s="4"/>
+      <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
@@ -2259,35 +2301,39 @@
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E62" s="5">
+        <v>53</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G62" s="7">
         <v>42138</v>
       </c>
-      <c r="F62" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G62" s="7">
-        <v>42139</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D63" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="E63" s="5">
-        <v>42137</v>
-      </c>
-      <c r="F63" s="4"/>
-      <c r="G63" s="3"/>
+        <v>42138</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G63" s="7">
+        <v>42139</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
@@ -2295,30 +2341,28 @@
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D64" s="4"/>
       <c r="E64" s="5">
-        <v>42138</v>
+        <v>42137</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="4" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E65" s="5">
-        <v>42348</v>
+        <v>42138</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="3"/>
@@ -2329,69 +2373,69 @@
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="4" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E66" s="5">
-        <v>43017</v>
+        <v>42348</v>
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="3"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D67" s="4"/>
-      <c r="E67" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>90</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E67" s="5">
+        <v>43017</v>
+      </c>
+      <c r="F67" s="4"/>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G68" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G69" s="3"/>
+        <v>91</v>
+      </c>
+      <c r="G69" s="7">
+        <v>42146</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
@@ -2399,13 +2443,15 @@
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="4" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F70" s="4"/>
+      <c r="F70" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2414,275 +2460,273 @@
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F71" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="F71" s="4"/>
       <c r="G71" s="3"/>
     </row>
-    <row r="72" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E72" s="5">
-        <v>42146</v>
-      </c>
-      <c r="F72" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="D72" s="4"/>
+      <c r="E72" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="G72" s="3"/>
     </row>
-    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="4" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E73" s="5">
-        <v>42163</v>
+        <v>42146</v>
       </c>
       <c r="F73" s="4"/>
       <c r="G73" s="3"/>
     </row>
-    <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="4" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E74" s="5">
-        <v>42066</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G74" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>42163</v>
+      </c>
+      <c r="F74" s="4"/>
+      <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E75" s="5">
-        <v>42023</v>
+        <v>42066</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G75" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D76" s="4"/>
-      <c r="E76" s="5" t="s">
-        <v>38</v>
+        <v>51</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E76" s="5">
+        <v>42023</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G76" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="4" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="G77" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="4" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="D78" s="4"/>
-      <c r="E78" s="5"/>
+      <c r="E78" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="F78" s="4" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="G78" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E79" s="5">
-        <v>42188</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D79" s="4"/>
+      <c r="E79" s="5"/>
       <c r="F79" s="4" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="G79" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>113</v>
+        <v>60</v>
       </c>
       <c r="E80" s="5">
-        <v>42193</v>
+        <v>42188</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G80" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="E81" s="5">
-        <v>42256</v>
+        <v>42193</v>
       </c>
       <c r="F81" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G81" s="7">
-        <v>42380</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="4" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E82" s="5">
-        <v>42472</v>
+        <v>42256</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G82" s="7"/>
-    </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="G82" s="7">
+        <v>42380</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E83" s="5">
+        <v>42472</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G83" s="7"/>
+    </row>
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B84" s="3"/>
+      <c r="C84" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D83" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E83" s="5">
+      <c r="D84" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E84" s="5">
         <v>43238</v>
       </c>
-      <c r="F83" s="4"/>
-      <c r="G83" s="7"/>
-    </row>
-    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B84" s="3"/>
-      <c r="C84" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D84" s="4"/>
-      <c r="E84" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="F84" s="4"/>
-      <c r="G84" s="3"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G84" s="7"/>
+    </row>
+    <row r="85" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B85" s="3"/>
-      <c r="C85" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E85" s="5">
-        <v>42157</v>
+      <c r="C85" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D85" s="4"/>
+      <c r="E85" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F85" s="4"/>
       <c r="G85" s="3"/>
@@ -2693,50 +2737,50 @@
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D86" s="4"/>
-      <c r="E86" s="5" t="s">
-        <v>38</v>
+        <v>99</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E86" s="5">
+        <v>42157</v>
       </c>
       <c r="F86" s="4"/>
       <c r="G86" s="3"/>
     </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F87" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G87" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F87" s="4"/>
+      <c r="G87" s="3"/>
+    </row>
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E88" s="5">
-        <v>42135</v>
-      </c>
-      <c r="F88" s="4"/>
-      <c r="G88" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="D88" s="4"/>
+      <c r="E88" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G88" s="7">
+        <v>43194</v>
+      </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
@@ -2744,28 +2788,24 @@
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="4" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="E89" s="5">
-        <v>42205</v>
-      </c>
-      <c r="F89" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G89" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>42135</v>
+      </c>
+      <c r="F89" s="4"/>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="4" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>115</v>
@@ -2774,107 +2814,133 @@
         <v>42205</v>
       </c>
       <c r="F90" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G90" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="C91" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E91" s="5">
+        <v>42205</v>
+      </c>
+      <c r="F91" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="G90" s="3" t="s">
+      <c r="G91" s="3" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G90"/>
-  <conditionalFormatting sqref="C79:C82 C74:C77 C3:C13 C15 C54:C56 C31:C35 C66:C72 C22:C24 C84:C88 C20 C58:C64 C26 C28:C29 C37:C52">
-    <cfRule type="expression" dxfId="19" priority="26">
+  <autoFilter ref="A2:G91"/>
+  <conditionalFormatting sqref="C80:C83 C75:C78 C3:C13 C15 C55:C57 C32:C36 C67:C73 C23:C25 C85:C89 C21 C59:C65 C27 C29:C30 C38:C53">
+    <cfRule type="expression" dxfId="19" priority="27">
       <formula>ISBLANK($G3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C73">
-    <cfRule type="expression" dxfId="18" priority="21">
-      <formula>ISBLANK($G73)</formula>
+  <conditionalFormatting sqref="C74">
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>ISBLANK($G74)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C78">
-    <cfRule type="expression" dxfId="17" priority="20">
-      <formula>ISBLANK($G78)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C89">
-    <cfRule type="expression" dxfId="16" priority="19">
-      <formula>ISBLANK($G89)</formula>
+  <conditionalFormatting sqref="C79">
+    <cfRule type="expression" dxfId="17" priority="21">
+      <formula>ISBLANK($G79)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="expression" dxfId="15" priority="18">
+    <cfRule type="expression" dxfId="16" priority="20">
       <formula>ISBLANK($G90)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="14" priority="17">
-      <formula>ISBLANK($G21)</formula>
+  <conditionalFormatting sqref="C91">
+    <cfRule type="expression" dxfId="15" priority="19">
+      <formula>ISBLANK($G91)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="expression" dxfId="14" priority="18">
+      <formula>ISBLANK($G22)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="13" priority="17">
       <formula>ISBLANK($G14)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="12" priority="15">
-      <formula>ISBLANK($G53)</formula>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>ISBLANK($G54)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>ISBLANK($G30)</formula>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="expression" dxfId="11" priority="14">
+      <formula>ISBLANK($G31)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>ISBLANK($G65)</formula>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" dxfId="10" priority="13">
+      <formula>ISBLANK($G66)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C83">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>ISBLANK($G83)</formula>
+  <conditionalFormatting sqref="C84">
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>ISBLANK($G84)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>ISBLANK($G57)</formula>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>ISBLANK($G58)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>ISBLANK($G25)</formula>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>ISBLANK($G26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>ISBLANK($G16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>ISBLANK($G18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>ISBLANK($G17)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>ISBLANK($G27)</formula>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>ISBLANK($G28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>ISBLANK($G19)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>ISBLANK($G36)</formula>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>ISBLANK($G37)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>ISBLANK($G20)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2882,6 +2948,7 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;F&amp;R&amp;D &amp;T</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
All changes 10sep2019-11sep2020 (git corrupted so details only available in network-backup repo)
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Old Home Drives\ado\ian\network\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\network\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="versions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$96</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'To do'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -45,6 +45,30 @@
 label def trt 1 "SK" 2 "AtPA" 3 "tPA" 6 "Ret"  5 "Ten"  4 "SK+tPA"  7 "UK"  8 "ASPAC", modify
 network setup r n, studyvar(study) trtvar(trt) nocodes
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ian White:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+need to print a warning that network meta will fail (but network map may succeed)</t>
         </r>
       </text>
     </comment>
@@ -100,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="196">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -659,9 +683,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Failes from pairs format with nested treatment names</t>
-  </si>
-  <si>
     <t>Ewelina</t>
   </si>
   <si>
@@ -684,6 +705,21 @@
   </si>
   <si>
     <t>fixed</t>
+  </si>
+  <si>
+    <t>Fails from pairs format with nested treatment names</t>
+  </si>
+  <si>
+    <t>Federico Tedeschi</t>
+  </si>
+  <si>
+    <t>also found with if (see email)</t>
+  </si>
+  <si>
+    <t>display study names if studyvar is labelled numeric</t>
+  </si>
+  <si>
+    <t>Victor Oguoma</t>
   </si>
 </sst>
 </file>
@@ -1270,13 +1306,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomRight" activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,10 +1668,10 @@
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E19" s="19">
         <v>43593</v>
@@ -1649,7 +1685,7 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>60</v>
@@ -1795,10 +1831,10 @@
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" s="18" t="s">
         <v>183</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>184</v>
       </c>
       <c r="E28" s="19">
         <v>43593</v>
@@ -1861,7 +1897,7 @@
         <v>43017</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G31" s="8">
         <v>43712</v>
@@ -1962,10 +1998,10 @@
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E37" s="19">
         <v>43593</v>
@@ -2346,7 +2382,7 @@
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>60</v>
@@ -2625,30 +2661,30 @@
       <c r="F75" s="4"/>
       <c r="G75" s="3"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>60</v>
+        <v>192</v>
       </c>
       <c r="E76" s="5">
-        <v>43672</v>
+        <v>44041</v>
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="3"/>
     </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>60</v>
@@ -2659,241 +2695,243 @@
       <c r="F77" s="4"/>
       <c r="G77" s="3"/>
     </row>
-    <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="4" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E78" s="5">
-        <v>42066</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G78" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>43672</v>
+      </c>
+      <c r="F78" s="4"/>
+      <c r="G78" s="3"/>
+    </row>
+    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E79" s="5">
-        <v>42023</v>
+        <v>42066</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G79" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D80" s="4"/>
-      <c r="E80" s="5" t="s">
-        <v>38</v>
+        <v>51</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E80" s="5">
+        <v>42023</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G80" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="4" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="G81" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="4" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="D82" s="4"/>
-      <c r="E82" s="5"/>
+      <c r="E82" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="F82" s="4" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="G82" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E83" s="5">
-        <v>42188</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D83" s="4"/>
+      <c r="E83" s="5"/>
       <c r="F83" s="4" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="G83" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>113</v>
+        <v>60</v>
       </c>
       <c r="E84" s="5">
-        <v>42193</v>
+        <v>42188</v>
       </c>
       <c r="F84" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G84" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="E85" s="5">
-        <v>42256</v>
+        <v>42193</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G85" s="7">
-        <v>42380</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="4" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E86" s="5">
-        <v>42472</v>
+        <v>42256</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G86" s="7"/>
-    </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="G86" s="7">
+        <v>42380</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E87" s="5">
+        <v>42472</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G87" s="7"/>
+    </row>
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="C88" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D87" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E87" s="5">
+      <c r="D88" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E88" s="5">
         <v>43238</v>
       </c>
-      <c r="F87" s="4"/>
-      <c r="G87" s="7"/>
-    </row>
-    <row r="88" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B88" s="3"/>
-      <c r="C88" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D88" s="4"/>
-      <c r="E88" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="F88" s="4"/>
-      <c r="G88" s="3"/>
+      <c r="G88" s="7"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="4" t="s">
-        <v>99</v>
+        <v>194</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>50</v>
+        <v>195</v>
       </c>
       <c r="E89" s="5">
-        <v>42157</v>
+        <v>44084</v>
       </c>
       <c r="F89" s="4"/>
-      <c r="G89" s="3"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G89" s="7"/>
+    </row>
+    <row r="90" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B90" s="3"/>
-      <c r="C90" s="4" t="s">
-        <v>24</v>
+      <c r="C90" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="5" t="s">
@@ -2902,174 +2940,211 @@
       <c r="F90" s="4"/>
       <c r="G90" s="3"/>
     </row>
-    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D91" s="4"/>
-      <c r="E91" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F91" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G91" s="7">
-        <v>43194</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E91" s="5">
+        <v>42157</v>
+      </c>
+      <c r="F91" s="4"/>
+      <c r="G91" s="3"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E92" s="5">
-        <v>42135</v>
+        <v>24</v>
+      </c>
+      <c r="D92" s="4"/>
+      <c r="E92" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F92" s="4"/>
       <c r="G92" s="3"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E93" s="5">
-        <v>42205</v>
+        <v>26</v>
+      </c>
+      <c r="D93" s="4"/>
+      <c r="E93" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F93" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G93" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E94" s="5">
+        <v>42135</v>
+      </c>
+      <c r="F94" s="4"/>
+      <c r="G94" s="3"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B95" s="3"/>
+      <c r="C95" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E95" s="5">
+        <v>42205</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G95" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B96" s="3"/>
+      <c r="C96" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D96" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E94" s="5">
+      <c r="E96" s="5">
         <v>42205</v>
       </c>
-      <c r="F94" s="4" t="s">
+      <c r="F96" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="G94" s="3" t="s">
+      <c r="G96" s="3" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G94"/>
-  <conditionalFormatting sqref="C83:C86 C78:C81 C3:C13 C15 C55:C57 C32:C36 C68:C74 C23:C25 C88:C92 C21 C60:C66 C27 C29:C30 C38:C53">
-    <cfRule type="expression" dxfId="23" priority="31">
+  <autoFilter ref="A2:G96"/>
+  <conditionalFormatting sqref="C84:C87 C79:C82 C3:C13 C15 C55:C57 C32:C36 C68:C74 C23:C25 C90:C94 C21 C60:C66 C27 C29:C30 C38:C53">
+    <cfRule type="expression" dxfId="23" priority="32">
       <formula>ISBLANK($G3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C75">
-    <cfRule type="expression" dxfId="22" priority="26">
-      <formula>ISBLANK($G75)</formula>
+  <conditionalFormatting sqref="C76">
+    <cfRule type="expression" dxfId="22" priority="27">
+      <formula>ISBLANK($G76)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82">
-    <cfRule type="expression" dxfId="21" priority="25">
-      <formula>ISBLANK($G82)</formula>
+  <conditionalFormatting sqref="C83">
+    <cfRule type="expression" dxfId="21" priority="26">
+      <formula>ISBLANK($G83)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C93">
-    <cfRule type="expression" dxfId="20" priority="24">
-      <formula>ISBLANK($G93)</formula>
+  <conditionalFormatting sqref="C95">
+    <cfRule type="expression" dxfId="20" priority="25">
+      <formula>ISBLANK($G95)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C94">
-    <cfRule type="expression" dxfId="19" priority="23">
-      <formula>ISBLANK($G94)</formula>
+  <conditionalFormatting sqref="C96">
+    <cfRule type="expression" dxfId="19" priority="24">
+      <formula>ISBLANK($G96)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="18" priority="23">
       <formula>ISBLANK($G22)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="17" priority="22">
       <formula>ISBLANK($G14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="16" priority="21">
       <formula>ISBLANK($G54)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="14" priority="17">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>ISBLANK($G67)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C87">
-    <cfRule type="expression" dxfId="13" priority="15">
-      <formula>ISBLANK($G87)</formula>
+  <conditionalFormatting sqref="C88:C89">
+    <cfRule type="expression" dxfId="14" priority="16">
+      <formula>ISBLANK($G88)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>ISBLANK($G58)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>ISBLANK($G26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>ISBLANK($G16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>ISBLANK($G18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>ISBLANK($G17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>ISBLANK($G28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>ISBLANK($G19)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>ISBLANK($G37)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C78">
     <cfRule type="expression" dxfId="5" priority="6">
-      <formula>ISBLANK($G37)</formula>
+      <formula>ISBLANK($G78)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
@@ -3077,24 +3152,24 @@
       <formula>ISBLANK($G77)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
+  <conditionalFormatting sqref="C59">
     <cfRule type="expression" dxfId="3" priority="4">
-      <formula>ISBLANK($G76)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="2" priority="3">
       <formula>ISBLANK($G59)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>ISBLANK($G20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>ISBLANK($G31)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C75">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ISBLANK($G31)</formula>
+      <formula>ISBLANK($G75)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Start of major update: revision to network setup
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9948655-2AC7-40FB-A9C5-A2088CB20B41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA97A72-901E-4DB6-B403-08E6FA020423}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17040" yWindow="9180" windowWidth="21255" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6390" yWindow="3630" windowWidth="10260" windowHeight="10005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To do" sheetId="1" r:id="rId1"/>
     <sheet name="versions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$96</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'To do'!$1:$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -30,7 +41,7 @@
     <author>Ian White</author>
   </authors>
   <commentList>
-    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="C26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C58" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="C57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C59" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="C58" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -120,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C60" authorId="0" shapeId="0" xr:uid="{7EF1E235-E37C-4ECD-A38A-3DB1D152723C}">
+    <comment ref="C59" authorId="0" shapeId="0" xr:uid="{7EF1E235-E37C-4ECD-A38A-3DB1D152723C}">
       <text>
         <r>
           <rPr>
@@ -148,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="205">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -698,9 +709,6 @@
     <t>Michael Kundi</t>
   </si>
   <si>
-    <t>anova within compute_df seems to hang when I tried it with 2000 studies</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -756,6 +764,24 @@
   </si>
   <si>
     <t>Peter G</t>
+  </si>
+  <si>
+    <t>wrote network_list</t>
+  </si>
+  <si>
+    <t>I can't reproduce this error</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>inform correspondent</t>
+  </si>
+  <si>
+    <t>Changed error to "Sorry, treatment codes must only include alphanumeric characters"</t>
+  </si>
+  <si>
+    <t>Changed compute_df to avoid anova</t>
   </si>
 </sst>
 </file>
@@ -893,9 +919,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -915,6 +938,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1389,13 +1415,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A99" sqref="A99"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,18 +1436,18 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>36</v>
@@ -1438,8 +1464,11 @@
       <c r="G2" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1458,7 +1487,7 @@
         <v>42135</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1477,7 +1506,7 @@
         <v>42135</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1496,7 +1525,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1517,7 +1546,7 @@
         <v>42076</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1538,7 +1567,7 @@
         <v>42163</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1552,15 +1581,19 @@
       <c r="E8" s="5">
         <v>42166</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G8" s="7">
+        <v>44293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="15" t="s">
         <v>102</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1572,7 +1605,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -1593,7 +1626,7 @@
         <v>42191</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
@@ -1614,7 +1647,7 @@
         <v>42191</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -1628,10 +1661,14 @@
       <c r="E12" s="5">
         <v>42242</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F12" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G12" s="7">
+        <v>44293</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1650,7 +1687,7 @@
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1671,7 +1708,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -1692,12 +1729,12 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="22" t="s">
         <v>175</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -1706,15 +1743,19 @@
       <c r="E16" s="5">
         <v>43250</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G16" s="7">
+        <v>44293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="17" t="s">
         <v>178</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -1723,69 +1764,89 @@
       <c r="E17" s="5">
         <v>43085</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F17" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G17" s="7">
+        <v>44293</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="5">
-        <v>43531</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" s="18">
+        <v>43593</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G18" s="7">
+        <v>44293</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="E19" s="19">
-        <v>43593</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="18">
+        <v>43712</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G19" s="7">
+        <v>44293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="19">
-        <v>43712</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="5">
+        <v>42045</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>43</v>
@@ -1793,20 +1854,16 @@
       <c r="E21" s="5">
         <v>42045</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="4"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>43</v>
@@ -1814,22 +1871,24 @@
       <c r="E22" s="5">
         <v>42045</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="5">
-        <v>42045</v>
+        <v>3</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>66</v>
@@ -1838,210 +1897,210 @@
         <v>42135</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G24" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="5">
+        <v>42262</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="4" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>123</v>
+        <v>60</v>
       </c>
       <c r="E25" s="5">
-        <v>42262</v>
+        <v>43238</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="4" t="s">
-        <v>173</v>
+      <c r="C26" s="15" t="s">
+        <v>177</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E26" s="5">
-        <v>43238</v>
+        <v>43356</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="5">
-        <v>43356</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="E28" s="19">
+      <c r="B27" s="16"/>
+      <c r="C27" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="E27" s="18">
         <v>43593</v>
       </c>
-      <c r="F28" s="18"/>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="17"/>
+      <c r="G27" s="19"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="8">
+        <v>42077</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5" t="s">
-        <v>38</v>
+        <v>126</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="5">
+        <v>42314</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="G29" s="8">
-        <v>42077</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42964</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="4" t="s">
-        <v>126</v>
+      <c r="C30" s="17" t="s">
+        <v>148</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E30" s="5">
-        <v>42314</v>
+        <v>43017</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>137</v>
+        <v>188</v>
       </c>
       <c r="G30" s="8">
-        <v>42964</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43712</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="5">
-        <v>43017</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G31" s="8">
-        <v>43712</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="7">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="5">
+        <v>41914</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G33" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="4" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E34" s="5">
-        <v>41914</v>
+        <v>42137</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>60</v>
@@ -2050,51 +2109,43 @@
         <v>42137</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="G35" s="7">
+        <v>42139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="5">
-        <v>42137</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G36" s="7">
-        <v>42139</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="E36" s="18">
+        <v>43593</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="19"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B37" s="3"/>
-      <c r="C37" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="E37" s="19">
-        <v>43593</v>
-      </c>
-      <c r="F37" s="18"/>
-      <c r="G37" s="20"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
@@ -2105,7 +2156,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
@@ -2116,14 +2167,20 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
+      <c r="C40" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="3"/>
+      <c r="F40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G40" s="7">
+        <v>42138</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -2131,15 +2188,17 @@
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="5"/>
+      <c r="E41" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="F41" s="4" t="s">
         <v>73</v>
       </c>
       <c r="G41" s="7">
-        <v>42138</v>
+        <v>42137</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2148,18 +2207,14 @@
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="4" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G42" s="7">
-        <v>42137</v>
-      </c>
+      <c r="F42" s="4"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -2167,7 +2222,7 @@
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="5" t="s">
@@ -2176,20 +2231,26 @@
       <c r="F43" s="4"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="5">
+        <v>41934</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G44" s="7">
+        <v>42138</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
@@ -2197,7 +2258,7 @@
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>47</v>
@@ -2218,59 +2279,59 @@
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D46" s="4"/>
       <c r="E46" s="5">
-        <v>41934</v>
+        <v>42135</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G46" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="5">
-        <v>42135</v>
+        <v>63</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G47" s="7">
         <v>42137</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>38</v>
+        <v>60</v>
+      </c>
+      <c r="E48" s="5">
+        <v>42137</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G48" s="7">
-        <v>42137</v>
+        <v>42138</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2279,7 +2340,7 @@
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>60</v>
@@ -2288,10 +2349,10 @@
         <v>42137</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G49" s="7">
-        <v>42138</v>
+        <v>42137</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2300,68 +2361,64 @@
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="4" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="E50" s="5">
-        <v>42137</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G50" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42176</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="7"/>
+    </row>
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="E51" s="5">
-        <v>42176</v>
+        <v>42179</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="4" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="E52" s="5">
-        <v>42179</v>
+        <v>42242</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="4" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="E53" s="5">
-        <v>42242</v>
+        <v>42348</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="7"/>
@@ -2372,16 +2429,20 @@
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="4" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E54" s="5">
-        <v>42348</v>
-      </c>
-      <c r="F54" s="4"/>
-      <c r="G54" s="7"/>
+        <v>42619</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G54" s="7">
+        <v>43194</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
@@ -2389,28 +2450,28 @@
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E55" s="5">
-        <v>42619</v>
+        <v>42915</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G55" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="G55" s="5">
+        <v>42915</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>60</v>
@@ -2418,26 +2479,22 @@
       <c r="E56" s="5">
         <v>42915</v>
       </c>
-      <c r="F56" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G56" s="5">
-        <v>42915</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="F56" s="4"/>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B57" s="3"/>
-      <c r="C57" s="4" t="s">
-        <v>136</v>
+      <c r="C57" s="15" t="s">
+        <v>176</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E57" s="5">
-        <v>42915</v>
+        <v>43228</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="5"/>
@@ -2447,14 +2504,14 @@
         <v>12</v>
       </c>
       <c r="B58" s="3"/>
-      <c r="C58" s="16" t="s">
-        <v>176</v>
+      <c r="C58" s="17" t="s">
+        <v>186</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E58" s="5">
-        <v>43228</v>
+        <v>43672</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="5"/>
@@ -2464,34 +2521,30 @@
         <v>12</v>
       </c>
       <c r="B59" s="3"/>
-      <c r="C59" s="18" t="s">
-        <v>187</v>
+      <c r="C59" s="17" t="s">
+        <v>194</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E59" s="5">
-        <v>43672</v>
+        <v>44144</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="5"/>
     </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B60" s="3"/>
-      <c r="C60" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E60" s="5">
-        <v>44144</v>
-      </c>
+      <c r="C60" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="5"/>
       <c r="F60" s="4"/>
-      <c r="G60" s="5"/>
+      <c r="G60" s="3"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
@@ -2499,10 +2552,12 @@
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D61" s="4"/>
-      <c r="E61" s="5"/>
+      <c r="E61" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="F61" s="4"/>
       <c r="G61" s="3"/>
     </row>
@@ -2512,7 +2567,7 @@
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="5" t="s">
@@ -2527,14 +2582,18 @@
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="4" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F63" s="4"/>
-      <c r="G63" s="3"/>
+      <c r="F63" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G63" s="7">
+        <v>42138</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
@@ -2542,39 +2601,35 @@
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D64" s="4"/>
-      <c r="E64" s="5" t="s">
-        <v>38</v>
+        <v>84</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E64" s="5">
+        <v>42138</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="G64" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D65" s="4"/>
       <c r="E65" s="5">
-        <v>42138</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G65" s="7">
-        <v>42139</v>
-      </c>
+        <v>42137</v>
+      </c>
+      <c r="F65" s="4"/>
+      <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
@@ -2582,28 +2637,30 @@
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D66" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="E66" s="5">
-        <v>42137</v>
+        <v>42138</v>
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="4" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E67" s="5">
-        <v>42138</v>
+        <v>42348</v>
       </c>
       <c r="F67" s="4"/>
       <c r="G67" s="3"/>
@@ -2614,69 +2671,69 @@
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E68" s="5">
-        <v>42348</v>
+        <v>43017</v>
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="3"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E69" s="5">
-        <v>43017</v>
-      </c>
-      <c r="F69" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="D69" s="4"/>
+      <c r="E69" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="G69" s="3"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G70" s="3"/>
-    </row>
-    <row r="71" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="G70" s="7">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G71" s="7">
-        <v>42146</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
@@ -2684,15 +2741,13 @@
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F72" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="F72" s="4"/>
       <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2701,45 +2756,47 @@
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F73" s="4"/>
+      <c r="F73" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="G73" s="3"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D74" s="4"/>
-      <c r="E74" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>90</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E74" s="5">
+        <v>42146</v>
+      </c>
+      <c r="F74" s="4"/>
       <c r="G74" s="3"/>
     </row>
-    <row r="75" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="4" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E75" s="5">
-        <v>42146</v>
+        <v>42163</v>
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="3"/>
@@ -2750,35 +2807,35 @@
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
-        <v>100</v>
+        <v>191</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="E76" s="5">
-        <v>42163</v>
+        <v>44041</v>
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="3"/>
     </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="4" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>191</v>
+        <v>60</v>
       </c>
       <c r="E77" s="5">
-        <v>44041</v>
+        <v>43672</v>
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="3"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>17</v>
       </c>
@@ -2795,249 +2852,249 @@
       <c r="F78" s="4"/>
       <c r="G78" s="3"/>
     </row>
-    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="4" t="s">
-        <v>186</v>
+        <v>49</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E79" s="5">
-        <v>43672</v>
-      </c>
-      <c r="F79" s="4"/>
-      <c r="G79" s="3"/>
-    </row>
-    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>42066</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G79" s="7">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E80" s="5">
-        <v>42066</v>
+        <v>42023</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G80" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E81" s="5">
-        <v>42023</v>
+        <v>82</v>
+      </c>
+      <c r="D81" s="4"/>
+      <c r="E81" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G81" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="4" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="G82" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="4" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="D83" s="4"/>
-      <c r="E83" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="E83" s="5"/>
       <c r="F83" s="4" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="G83" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D84" s="4"/>
-      <c r="E84" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E84" s="5">
+        <v>42188</v>
+      </c>
       <c r="F84" s="4" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="G84" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="4" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="E85" s="5">
-        <v>42188</v>
+        <v>42193</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G85" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="4" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>113</v>
+        <v>60</v>
       </c>
       <c r="E86" s="5">
-        <v>42193</v>
+        <v>42256</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G86" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42380</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="4" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E87" s="5">
-        <v>42256</v>
+        <v>42472</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G87" s="7">
-        <v>42380</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="G87" s="7"/>
+    </row>
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="4" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E88" s="5">
-        <v>42472</v>
-      </c>
-      <c r="F88" s="4" t="s">
-        <v>172</v>
-      </c>
+        <v>43238</v>
+      </c>
+      <c r="F88" s="4"/>
       <c r="G88" s="7"/>
     </row>
-    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="4" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>60</v>
+        <v>193</v>
       </c>
       <c r="E89" s="5">
-        <v>43238</v>
+        <v>44084</v>
       </c>
       <c r="F89" s="4"/>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>22</v>
+        <v>195</v>
       </c>
       <c r="B90" s="3"/>
-      <c r="C90" s="4" t="s">
-        <v>193</v>
+      <c r="C90" s="21" t="s">
+        <v>196</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>194</v>
+        <v>60</v>
       </c>
       <c r="E90" s="5">
-        <v>44084</v>
+        <v>44214</v>
       </c>
       <c r="F90" s="4"/>
-      <c r="G90" s="7"/>
-    </row>
-    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G90" s="3"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>196</v>
+        <v>23</v>
       </c>
       <c r="B91" s="3"/>
-      <c r="C91" s="22" t="s">
-        <v>197</v>
+      <c r="C91" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E91" s="5">
-        <v>44214</v>
+        <v>42157</v>
       </c>
       <c r="F91" s="4"/>
       <c r="G91" s="3"/>
@@ -3048,50 +3105,50 @@
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E92" s="5">
-        <v>42157</v>
+        <v>24</v>
+      </c>
+      <c r="D92" s="4"/>
+      <c r="E92" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F92" s="4"/>
       <c r="G92" s="3"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F93" s="4"/>
-      <c r="G93" s="3"/>
-    </row>
-    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F93" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G93" s="7">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D94" s="4"/>
-      <c r="E94" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F94" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G94" s="7">
-        <v>43194</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E94" s="5">
+        <v>42135</v>
+      </c>
+      <c r="F94" s="4"/>
+      <c r="G94" s="3"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
@@ -3099,24 +3156,28 @@
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="4" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="E95" s="5">
-        <v>42135</v>
-      </c>
-      <c r="F95" s="4"/>
-      <c r="G95" s="3"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42205</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G95" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="4" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>115</v>
@@ -3125,80 +3186,59 @@
         <v>42205</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G96" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="4" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>115</v>
+        <v>198</v>
       </c>
       <c r="E97" s="5">
-        <v>42205</v>
-      </c>
-      <c r="F97" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G97" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E98" s="5">
         <v>44278</v>
       </c>
-      <c r="F98" s="4"/>
-      <c r="G98" s="3"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G97" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="C85:C88 C80:C83 C3:C13 C15 C55:C57 C32:C36 C69:C75 C23:C25 C91:C95 C21 C61:C67 C27 C29:C30 C38:C53">
+  <autoFilter ref="A2:G96" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="C84:C87 C79:C82 C3:C13 C15 C54:C56 C31:C35 C68:C74 C22:C24 C90:C94 C20 C60:C66 C26 C28:C29 C37:C52">
     <cfRule type="expression" dxfId="25" priority="34">
       <formula>ISBLANK($G3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
+  <conditionalFormatting sqref="C76">
     <cfRule type="expression" dxfId="24" priority="29">
-      <formula>ISBLANK($G77)</formula>
+      <formula>ISBLANK($G76)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C84">
+  <conditionalFormatting sqref="C83">
     <cfRule type="expression" dxfId="23" priority="28">
-      <formula>ISBLANK($G84)</formula>
+      <formula>ISBLANK($G83)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C95">
+    <cfRule type="expression" dxfId="22" priority="27">
+      <formula>ISBLANK($G95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C96">
-    <cfRule type="expression" dxfId="22" priority="27">
+    <cfRule type="expression" dxfId="21" priority="26">
       <formula>ISBLANK($G96)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C97">
-    <cfRule type="expression" dxfId="21" priority="26">
-      <formula>ISBLANK($G97)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
+  <conditionalFormatting sqref="C21">
     <cfRule type="expression" dxfId="20" priority="25">
-      <formula>ISBLANK($G22)</formula>
+      <formula>ISBLANK($G21)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
@@ -3206,29 +3246,29 @@
       <formula>ISBLANK($G14)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
+  <conditionalFormatting sqref="C53">
     <cfRule type="expression" dxfId="18" priority="23">
-      <formula>ISBLANK($G54)</formula>
+      <formula>ISBLANK($G53)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
+  <conditionalFormatting sqref="C67">
     <cfRule type="expression" dxfId="17" priority="20">
-      <formula>ISBLANK($G68)</formula>
+      <formula>ISBLANK($G67)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C89:C90">
+  <conditionalFormatting sqref="C88:C89">
     <cfRule type="expression" dxfId="16" priority="18">
-      <formula>ISBLANK($G89)</formula>
+      <formula>ISBLANK($G88)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
+  <conditionalFormatting sqref="C57">
     <cfRule type="expression" dxfId="15" priority="16">
-      <formula>ISBLANK($G58)</formula>
+      <formula>ISBLANK($G57)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
+  <conditionalFormatting sqref="C25">
     <cfRule type="expression" dxfId="14" priority="15">
-      <formula>ISBLANK($G26)</formula>
+      <formula>ISBLANK($G25)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
@@ -3236,69 +3276,64 @@
       <formula>ISBLANK($G16)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="12" priority="13">
-      <formula>ISBLANK($G18)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C17">
     <cfRule type="expression" dxfId="11" priority="12">
       <formula>ISBLANK($G17)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
+  <conditionalFormatting sqref="C27">
     <cfRule type="expression" dxfId="10" priority="11">
-      <formula>ISBLANK($G28)</formula>
+      <formula>ISBLANK($G27)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>ISBLANK($G18)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>ISBLANK($G36)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C78">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>ISBLANK($G78)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C77">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>ISBLANK($G77)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>ISBLANK($G58)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>ISBLANK($G19)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>ISBLANK($G37)</formula>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>ISBLANK($G30)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C79">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>ISBLANK($G79)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C78">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>ISBLANK($G78)</formula>
+  <conditionalFormatting sqref="C75">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>ISBLANK($G75)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>ISBLANK($G59)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>ISBLANK($G20)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>ISBLANK($G31)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>ISBLANK($G76)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>ISBLANK($G60)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C98">
+  <conditionalFormatting sqref="C97">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ISBLANK($G98)</formula>
+      <formula>ISBLANK($G97)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Improved error checks for network import from pairs format
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA97A72-901E-4DB6-B403-08E6FA020423}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FDDE37-04A5-471C-B48A-79249BA01229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6390" yWindow="3630" windowWidth="10260" windowHeight="10005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="209">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -363,9 +363,6 @@
   </si>
   <si>
     <t>done</t>
-  </si>
-  <si>
-    <t>discuss with Anna C</t>
   </si>
   <si>
     <t>discuss components and df in help file (&amp; in setup)</t>
@@ -421,9 +418,6 @@
   </si>
   <si>
     <t>checked; warning added to help file</t>
-  </si>
-  <si>
-    <t>only happened in one particular session - haven’t been able to replicate the problem</t>
   </si>
   <si>
     <t>corrected</t>
@@ -688,9 +682,6 @@
     <t>not sure how to do this without making labels too long.</t>
   </si>
   <si>
-    <t>Handle labelled treatments by (i) check they are consistently labelled; (ii) using labels</t>
-  </si>
-  <si>
     <t>cscript must test extraction using clear &amp; test of single-study design</t>
   </si>
   <si>
@@ -782,6 +773,27 @@
   </si>
   <si>
     <t>Changed compute_df to avoid anova</t>
+  </si>
+  <si>
+    <t>Handle labelled treatments by (i) checking they are consistently labelled; (ii) using labels</t>
+  </si>
+  <si>
+    <t>it's working</t>
+  </si>
+  <si>
+    <t>Added check &amp; error message (also for missing contrasts)</t>
+  </si>
+  <si>
+    <t>Labels are now used</t>
+  </si>
+  <si>
+    <t>I can't reproduce this error, but I've added a check to cscript</t>
+  </si>
+  <si>
+    <t>only happened in one particular session - haven’t been able to replicate the problem - treat as fixed</t>
+  </si>
+  <si>
+    <t>ignore?</t>
   </si>
 </sst>
 </file>
@@ -1418,10 +1430,10 @@
   <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1459,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>36</v>
@@ -1465,7 +1477,7 @@
         <v>34</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1552,16 +1564,16 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E7" s="5">
         <v>42157</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G7" s="7">
         <v>42163</v>
@@ -1573,7 +1585,7 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>60</v>
@@ -1582,7 +1594,7 @@
         <v>42166</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G8" s="7">
         <v>44293</v>
@@ -1594,7 +1606,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>60</v>
@@ -1611,7 +1623,7 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>60</v>
@@ -1620,7 +1632,7 @@
         <v>42191</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G10" s="7">
         <v>42191</v>
@@ -1632,7 +1644,7 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>60</v>
@@ -1641,7 +1653,7 @@
         <v>42191</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G11" s="7">
         <v>42191</v>
@@ -1653,7 +1665,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>60</v>
@@ -1662,7 +1674,7 @@
         <v>42242</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G12" s="7">
         <v>44293</v>
@@ -1674,7 +1686,7 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>60</v>
@@ -1683,7 +1695,7 @@
         <v>42256</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G13" s="7"/>
     </row>
@@ -1693,7 +1705,7 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>60</v>
@@ -1702,7 +1714,7 @@
         <v>42314</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G14" s="7">
         <v>43194</v>
@@ -1714,16 +1726,16 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E15" s="5">
         <v>42388</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G15" s="7">
         <v>43194</v>
@@ -1735,7 +1747,7 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>60</v>
@@ -1744,7 +1756,7 @@
         <v>43250</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G16" s="7">
         <v>44293</v>
@@ -1756,22 +1768,22 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="17" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E17" s="5">
         <v>43085</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G17" s="7">
         <v>44293</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1780,22 +1792,22 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E18" s="18">
         <v>43593</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G18" s="7">
         <v>44293</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1804,7 +1816,7 @@
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>60</v>
@@ -1813,7 +1825,7 @@
         <v>43712</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G19" s="7">
         <v>44293</v>
@@ -1825,7 +1837,7 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>43</v>
@@ -1845,8 +1857,8 @@
         <v>2</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="4" t="s">
-        <v>125</v>
+      <c r="C21" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>43</v>
@@ -1903,16 +1915,23 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E24" s="5">
         <v>42262</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="7"/>
+      <c r="F24" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G24" s="7">
+        <v>44293</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -1920,7 +1939,7 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="4" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>60</v>
@@ -1928,16 +1947,20 @@
       <c r="E25" s="5">
         <v>43238</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F25" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="G25" s="7">
+        <v>44293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="15" t="s">
-        <v>177</v>
+      <c r="C26" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>60</v>
@@ -1945,25 +1968,36 @@
       <c r="E26" s="5">
         <v>43356</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G26" s="7">
+        <v>44293</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="16"/>
       <c r="C27" s="17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E27" s="18">
         <v>43593</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="19"/>
+      <c r="F27" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G27" s="7">
+        <v>44293</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -1990,7 +2024,7 @@
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>60</v>
@@ -1999,7 +2033,7 @@
         <v>42314</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G29" s="8">
         <v>42964</v>
@@ -2011,7 +2045,7 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>60</v>
@@ -2020,7 +2054,7 @@
         <v>43017</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G30" s="8">
         <v>43712</v>
@@ -2071,17 +2105,17 @@
         <v>41914</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>68</v>
+        <v>208</v>
       </c>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>60</v>
@@ -2090,9 +2124,11 @@
         <v>42137</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G34" s="3"/>
+        <v>207</v>
+      </c>
+      <c r="G34" s="7">
+        <v>44293</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
@@ -2100,7 +2136,7 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>60</v>
@@ -2109,7 +2145,7 @@
         <v>42137</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G35" s="7">
         <v>42139</v>
@@ -2121,10 +2157,10 @@
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E36" s="18">
         <v>43593</v>
@@ -2171,12 +2207,12 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
       <c r="F40" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G40" s="7">
         <v>42138</v>
@@ -2188,14 +2224,14 @@
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G41" s="7">
         <v>42137</v>
@@ -2246,7 +2282,7 @@
         <v>41934</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G44" s="7">
         <v>42138</v>
@@ -2267,7 +2303,7 @@
         <v>41934</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G45" s="7">
         <v>42138</v>
@@ -2286,7 +2322,7 @@
         <v>42135</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G46" s="7">
         <v>42137</v>
@@ -2307,7 +2343,7 @@
         <v>38</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G47" s="7">
         <v>42137</v>
@@ -2319,7 +2355,7 @@
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>60</v>
@@ -2328,7 +2364,7 @@
         <v>42137</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G48" s="7">
         <v>42138</v>
@@ -2340,7 +2376,7 @@
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>60</v>
@@ -2349,7 +2385,7 @@
         <v>42137</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G49" s="7">
         <v>42137</v>
@@ -2361,10 +2397,10 @@
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E50" s="5">
         <v>42176</v>
@@ -2378,7 +2414,7 @@
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>60</v>
@@ -2395,10 +2431,10 @@
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E52" s="5">
         <v>42242</v>
@@ -2412,7 +2448,7 @@
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>60</v>
@@ -2429,7 +2465,7 @@
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>60</v>
@@ -2438,7 +2474,7 @@
         <v>42619</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G54" s="7">
         <v>43194</v>
@@ -2450,7 +2486,7 @@
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>60</v>
@@ -2459,7 +2495,7 @@
         <v>42915</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G55" s="5">
         <v>42915</v>
@@ -2471,7 +2507,7 @@
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>60</v>
@@ -2488,7 +2524,7 @@
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="15" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>60</v>
@@ -2505,7 +2541,7 @@
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>60</v>
@@ -2522,7 +2558,7 @@
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="17" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>60</v>
@@ -2601,7 +2637,7 @@
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>60</v>
@@ -2610,7 +2646,7 @@
         <v>42138</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G64" s="7">
         <v>42139</v>
@@ -2622,7 +2658,7 @@
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="5">
@@ -2637,7 +2673,7 @@
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>60</v>
@@ -2654,7 +2690,7 @@
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>60</v>
@@ -2671,7 +2707,7 @@
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>60</v>
@@ -2695,7 +2731,7 @@
         <v>38</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G69" s="3"/>
     </row>
@@ -2712,7 +2748,7 @@
         <v>38</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G70" s="7">
         <v>42146</v>
@@ -2731,7 +2767,7 @@
         <v>38</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G71" s="3"/>
     </row>
@@ -2763,7 +2799,7 @@
         <v>38</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G73" s="3"/>
     </row>
@@ -2773,7 +2809,7 @@
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>60</v>
@@ -2790,7 +2826,7 @@
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>60</v>
@@ -2807,10 +2843,10 @@
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E76" s="5">
         <v>44041</v>
@@ -2824,7 +2860,7 @@
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>60</v>
@@ -2841,7 +2877,7 @@
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>60</v>
@@ -2867,7 +2903,7 @@
         <v>42066</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G79" s="7">
         <v>42146</v>
@@ -2888,7 +2924,7 @@
         <v>42023</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G80" s="7">
         <v>42146</v>
@@ -2900,14 +2936,14 @@
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G81" s="7">
         <v>42146</v>
@@ -2938,12 +2974,12 @@
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="5"/>
       <c r="F83" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G83" s="7">
         <v>42146</v>
@@ -2955,7 +2991,7 @@
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>60</v>
@@ -2976,10 +3012,10 @@
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E85" s="5">
         <v>42193</v>
@@ -2997,7 +3033,7 @@
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>60</v>
@@ -3018,7 +3054,7 @@
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>60</v>
@@ -3027,7 +3063,7 @@
         <v>42472</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G87" s="7"/>
     </row>
@@ -3037,7 +3073,7 @@
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>60</v>
@@ -3054,10 +3090,10 @@
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E89" s="5">
         <v>44084</v>
@@ -3067,11 +3103,11 @@
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="21" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>60</v>
@@ -3088,7 +3124,7 @@
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>50</v>
@@ -3156,10 +3192,10 @@
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E95" s="5">
         <v>42205</v>
@@ -3177,19 +3213,19 @@
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E96" s="5">
         <v>42205</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3198,10 +3234,10 @@
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E97" s="5">
         <v>44278</v>
@@ -3364,67 +3400,67 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>142</v>
-      </c>
       <c r="C3" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D3" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="J3" s="13" t="s">
+      <c r="M3" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="N3" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="L3" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="M3" s="13" t="s">
+      <c r="O3" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="O3" s="13" t="s">
+      <c r="P3" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q3" s="13" t="s">
         <v>163</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -3433,7 +3469,7 @@
       </c>
       <c r="C5" s="10"/>
       <c r="L5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -3442,36 +3478,36 @@
       </c>
       <c r="C6" s="12"/>
       <c r="P6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" s="10">
         <v>42976</v>
       </c>
       <c r="C8" s="10"/>
       <c r="P8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B9" s="10">
         <v>43017</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -3482,15 +3518,15 @@
         <v>43105</v>
       </c>
       <c r="P10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvements to network meta: fixed option works in pairs format; also two bug fixes. Removed extra spaces in mvmeta call, hence many changes in testlog.
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FDDE37-04A5-471C-B48A-79249BA01229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89769C03-01B9-4590-B16A-74E172A94879}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6390" yWindow="3630" windowWidth="10260" windowHeight="10005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,120 +38,49 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Ian White</author>
+    <author>tc={C08FE597-3E36-4419-899A-40FB8D43C16F}</author>
+    <author>tc={EBD4C436-E631-4AF3-8DA4-6B56C6A448C0}</author>
+    <author>tc={ED6B4446-BECB-4AC2-AC74-C14778DF40D1}</author>
+    <author>tc={50F99A35-5AC1-458D-8F00-D63EFAC00865}</author>
   </authors>
   <commentList>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{C08FE597-3E36-4419-899A-40FB8D43C16F}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">use http://www.homepages.ucl.ac.uk/~rmjwiww/stata/meta/thromb.dta, clear
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    use http://www.homepages.ucl.ac.uk/~rmjwiww/stata/meta/thromb.dta, clear
 encode treat, gen(trt)
 drop treat
 label def trt 1 "SK" 2 "AtPA" 3 "tPA" 6 "Ret"  5 "Ten"  4 "SK+tPA"  7 "UK"  8 "ASPAC", modify
 network setup r n, studyvar(study) trtvar(trt) nocodes
 </t>
-        </r>
       </text>
     </comment>
-    <comment ref="C26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="C25" authorId="1" shapeId="0" xr:uid="{EBD4C436-E631-4AF3-8DA4-6B56C6A448C0}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ian White:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-need to print a warning that network meta will fail (but network map may succeed)</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    need to print a warning that network meta will fail (but network map may succeed)</t>
       </text>
     </comment>
-    <comment ref="C57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="C58" authorId="2" shapeId="0" xr:uid="{ED6B4446-BECB-4AC2-AC74-C14778DF40D1}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ian White:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    e.g.
+reg _y _trtdiff_C _trtdiff_D [aw=1/_stderr^2], mse1 noconstant</t>
       </text>
     </comment>
-    <comment ref="C58" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="C59" authorId="3" shapeId="0" xr:uid="{50F99A35-5AC1-458D-8F00-D63EFAC00865}">
       <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">e.g.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>reg _y _trtdiff_C _trtdiff_D [aw=1/_stderr^2], mse1 noconstant</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C59" authorId="0" shapeId="0" xr:uid="{7EF1E235-E37C-4ECD-A38A-3DB1D152723C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">e.g.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>reg _y _trtdiff_C _trtdiff_D [aw=1/_stderr^2], mse1 noconstant</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    e.g.
+reg _y _trtdiff_C _trtdiff_D [aw=1/_stderr^2], mse1 noconstant</t>
       </text>
     </comment>
   </commentList>
@@ -159,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="218">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -369,9 +298,6 @@
   </si>
   <si>
     <t>add to output "showing only study 1 as all studies are the same"?</t>
-  </si>
-  <si>
-    <t>sometimes networkplot gives an error 4020 "not an array" at the -twoway- statement - can solve this by -discard-</t>
   </si>
   <si>
     <t>doesn't respect vars() option - probably fine but might want to issue a warning?</t>
@@ -790,17 +716,47 @@
     <t>I can't reproduce this error, but I've added a check to cscript</t>
   </si>
   <si>
-    <t>only happened in one particular session - haven’t been able to replicate the problem - treat as fixed</t>
-  </si>
-  <si>
-    <t>ignore?</t>
+    <t>implemented</t>
+  </si>
+  <si>
+    <t>I can't reproduce this error.</t>
+  </si>
+  <si>
+    <t>ignore</t>
+  </si>
+  <si>
+    <t>as far as I can see, this is not a problem</t>
+  </si>
+  <si>
+    <t>Sometimes networkplot gives an error 4020 "not an array" at the -twoway- statement. See error_4020.do. I haven't identified why it happened, but I have been able to solve it using -discard-.</t>
+  </si>
+  <si>
+    <t>next time it happens, run -program dir-</t>
+  </si>
+  <si>
+    <t>no longer an issue in modern Stata</t>
+  </si>
+  <si>
+    <t>what?</t>
+  </si>
+  <si>
+    <t>I can't reproduce this</t>
+  </si>
+  <si>
+    <t>make all warnings appear with "warning" in red and rest not in red</t>
+  </si>
+  <si>
+    <t>fixed by examining e(constant) at l472</t>
+  </si>
+  <si>
+    <t>as far as I can see, this is not a problem, but I've made metavars robust to model failing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,14 +794,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -959,7 +908,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1101,6 +1055,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Ian White" id="{5D58C562-25D2-4493-B339-1D5F20B1863B}" userId="Ian White" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1422,18 +1382,42 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C16" personId="{5D58C562-25D2-4493-B339-1D5F20B1863B}" id="{C08FE597-3E36-4419-899A-40FB8D43C16F}">
+    <text xml:space="preserve">use http://www.homepages.ucl.ac.uk/~rmjwiww/stata/meta/thromb.dta, clear
+encode treat, gen(trt)
+drop treat
+label def trt 1 "SK" 2 "AtPA" 3 "tPA" 6 "Ret"  5 "Ten"  4 "SK+tPA"  7 "UK"  8 "ASPAC", modify
+network setup r n, studyvar(study) trtvar(trt) nocodes
+</text>
+  </threadedComment>
+  <threadedComment ref="C25" personId="{5D58C562-25D2-4493-B339-1D5F20B1863B}" id="{EBD4C436-E631-4AF3-8DA4-6B56C6A448C0}">
+    <text>need to print a warning that network meta will fail (but network map may succeed)</text>
+  </threadedComment>
+  <threadedComment ref="C58" personId="{5D58C562-25D2-4493-B339-1D5F20B1863B}" id="{ED6B4446-BECB-4AC2-AC74-C14778DF40D1}">
+    <text>e.g.
+reg _y _trtdiff_C _trtdiff_D [aw=1/_stderr^2], mse1 noconstant</text>
+  </threadedComment>
+  <threadedComment ref="C59" personId="{5D58C562-25D2-4493-B339-1D5F20B1863B}" id="{50F99A35-5AC1-458D-8F00-D63EFAC00865}">
+    <text>e.g.
+reg _y _trtdiff_C _trtdiff_D [aw=1/_stderr^2], mse1 noconstant</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomRight" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,7 +1443,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>36</v>
@@ -1477,7 +1461,7 @@
         <v>34</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1486,17 +1470,19 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="5">
+        <v>42045</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" s="7">
-        <v>42135</v>
+        <v>42076</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -1505,14 +1491,14 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" s="7">
         <v>42135</v>
@@ -1524,17 +1510,17 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>38</v>
+        <v>56</v>
+      </c>
+      <c r="G5" s="7">
+        <v>42135</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1543,19 +1529,19 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="E6" s="5">
-        <v>42045</v>
+        <v>42157</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="G6" s="7">
-        <v>42076</v>
+        <v>42163</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1564,19 +1550,19 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="E7" s="5">
-        <v>42157</v>
+        <v>42191</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>107</v>
       </c>
       <c r="G7" s="7">
-        <v>42163</v>
+        <v>42191</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1585,19 +1571,19 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E8" s="5">
-        <v>42166</v>
+        <v>42191</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>201</v>
+        <v>108</v>
       </c>
       <c r="G8" s="7">
-        <v>44293</v>
+        <v>42191</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1605,37 +1591,41 @@
         <v>1</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="15" t="s">
-        <v>100</v>
+      <c r="C9" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E9" s="5">
-        <v>42166</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="7"/>
+        <v>42314</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" s="7">
+        <v>43194</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>105</v>
+      <c r="C10" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="E10" s="5">
-        <v>42191</v>
+        <v>42388</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
       <c r="G10" s="7">
-        <v>42191</v>
+        <v>43194</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1644,19 +1634,19 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E11" s="5">
-        <v>42191</v>
+        <v>42166</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>109</v>
+        <v>200</v>
       </c>
       <c r="G11" s="7">
-        <v>42191</v>
+        <v>44293</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1665,7 +1655,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>60</v>
@@ -1674,7 +1664,7 @@
         <v>42242</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G12" s="7">
         <v>44293</v>
@@ -1685,39 +1675,44 @@
         <v>1</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
-        <v>118</v>
+      <c r="C13" s="22" t="s">
+        <v>171</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E13" s="5">
-        <v>42256</v>
+        <v>43250</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" s="7"/>
+        <v>196</v>
+      </c>
+      <c r="G13" s="7">
+        <v>44293</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="9" t="s">
-        <v>165</v>
+      <c r="C14" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>60</v>
+        <v>175</v>
       </c>
       <c r="E14" s="5">
-        <v>42314</v>
+        <v>43085</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>166</v>
+        <v>196</v>
       </c>
       <c r="G14" s="7">
-        <v>43194</v>
+        <v>44293</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1726,19 +1721,22 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E15" s="5">
-        <v>42388</v>
+        <v>178</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="E15" s="18">
+        <v>43593</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>167</v>
+        <v>196</v>
       </c>
       <c r="G15" s="7">
-        <v>43194</v>
+        <v>44293</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1746,17 +1744,17 @@
         <v>1</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="5">
-        <v>43250</v>
+      <c r="C16" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="18">
+        <v>43712</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G16" s="7">
         <v>44293</v>
@@ -1767,23 +1765,18 @@
         <v>1</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E17" s="5">
-        <v>43085</v>
+      <c r="C17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="G17" s="7">
-        <v>44293</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>199</v>
+        <v>57</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1791,23 +1784,20 @@
         <v>1</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E18" s="18">
-        <v>43593</v>
+      <c r="C18" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="5">
+        <v>42166</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="G18" s="7">
-        <v>44293</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>199</v>
+        <v>44294</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1815,21 +1805,19 @@
         <v>1</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="18">
-        <v>43712</v>
+      <c r="C19" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="5">
+        <v>42256</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="G19" s="7">
-        <v>44293</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1837,7 +1825,7 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>43</v>
@@ -1857,8 +1845,8 @@
         <v>2</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="15" t="s">
-        <v>123</v>
+      <c r="C21" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>43</v>
@@ -1866,8 +1854,12 @@
       <c r="E21" s="5">
         <v>42045</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="7"/>
+      <c r="F21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" s="7">
+        <v>42135</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1875,13 +1867,11 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="5">
-        <v>42045</v>
+        <v>3</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>66</v>
@@ -1896,17 +1886,22 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5" t="s">
-        <v>38</v>
+        <v>119</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="5">
+        <v>42262</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>66</v>
+        <v>202</v>
       </c>
       <c r="G23" s="7">
-        <v>42135</v>
+        <v>44293</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1915,22 +1910,19 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="4" t="s">
-        <v>120</v>
+        <v>201</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>121</v>
+        <v>60</v>
       </c>
       <c r="E24" s="5">
-        <v>42262</v>
+        <v>43238</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G24" s="7">
         <v>44293</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1938,66 +1930,63 @@
         <v>2</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="4" t="s">
-        <v>202</v>
+      <c r="C25" s="17" t="s">
+        <v>173</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E25" s="5">
-        <v>43238</v>
+        <v>43356</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G25" s="7">
         <v>44293</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="5">
-        <v>43356</v>
+        <v>185</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" s="18">
+        <v>43593</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G26" s="7">
         <v>44293</v>
       </c>
+      <c r="H26" s="1" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="27" spans="1:8" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E27" s="18">
-        <v>43593</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="G27" s="7">
-        <v>44293</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>199</v>
-      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="5">
+        <v>42045</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -2024,7 +2013,7 @@
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>60</v>
@@ -2033,7 +2022,7 @@
         <v>42314</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G29" s="8">
         <v>42964</v>
@@ -2045,7 +2034,7 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>60</v>
@@ -2054,7 +2043,7 @@
         <v>43017</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G30" s="8">
         <v>43712</v>
@@ -2090,32 +2079,34 @@
         <v>42135</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="4" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E33" s="5">
-        <v>41914</v>
+        <v>42137</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="G33" s="7">
+        <v>42139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="4" t="s">
-        <v>70</v>
+        <v>210</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>60</v>
@@ -2124,51 +2115,58 @@
         <v>42137</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="G34" s="7">
         <v>44293</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="4" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E35" s="5">
-        <v>42137</v>
+        <v>41914</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G35" s="7">
-        <v>42139</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="G35" s="19">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E36" s="18">
         <v>43593</v>
       </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="19"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="G36" s="19">
+        <v>44294</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>9</v>
       </c>
@@ -2179,7 +2177,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>10</v>
       </c>
@@ -2190,7 +2188,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>11</v>
       </c>
@@ -2201,34 +2199,36 @@
       <c r="F39" s="4"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="4" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D40" s="4"/>
-      <c r="E40" s="5"/>
+      <c r="E40" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="F40" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G40" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="5" t="s">
-        <v>38</v>
+      <c r="E41" s="5">
+        <v>42135</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>72</v>
@@ -2237,64 +2237,72 @@
         <v>42137</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="E42" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G42" s="7">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="5">
+        <v>42137</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G43" s="7">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E44" s="5">
-        <v>41934</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="5"/>
       <c r="F44" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G44" s="7">
         <v>42138</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>47</v>
@@ -2303,71 +2311,73 @@
         <v>41934</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G45" s="7">
         <v>42138</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="E46" s="5">
-        <v>42135</v>
+        <v>41934</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G46" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="4" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>38</v>
+        <v>60</v>
+      </c>
+      <c r="E47" s="5">
+        <v>42137</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G47" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E48" s="5">
-        <v>42137</v>
+        <v>42915</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G48" s="7">
-        <v>42138</v>
+        <v>132</v>
+      </c>
+      <c r="G48" s="5">
+        <v>42915</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2376,88 +2386,102 @@
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="4" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E49" s="5">
-        <v>42137</v>
+        <v>42619</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="G49" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E50" s="5">
-        <v>42176</v>
-      </c>
-      <c r="F50" s="4"/>
-      <c r="G50" s="7"/>
-    </row>
-    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G50" s="7">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="4" t="s">
-        <v>103</v>
+        <v>14</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="5">
-        <v>42179</v>
-      </c>
-      <c r="F51" s="4"/>
-      <c r="G51" s="7"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E51" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G51" s="7">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="4" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E52" s="5">
-        <v>42242</v>
-      </c>
-      <c r="F52" s="4"/>
-      <c r="G52" s="7"/>
-    </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42176</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G52" s="7">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="4" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E53" s="5">
-        <v>42348</v>
-      </c>
-      <c r="F53" s="4"/>
-      <c r="G53" s="7"/>
+        <v>42179</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G53" s="7">
+        <v>44294</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
@@ -2465,19 +2489,19 @@
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="4" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="E54" s="5">
-        <v>42619</v>
+        <v>42242</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>151</v>
+        <v>212</v>
       </c>
       <c r="G54" s="7">
-        <v>43194</v>
+        <v>44294</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2486,19 +2510,19 @@
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E55" s="5">
-        <v>42915</v>
+        <v>42348</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G55" s="5">
-        <v>42915</v>
+        <v>213</v>
+      </c>
+      <c r="G55" s="7">
+        <v>44294</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2507,7 +2531,7 @@
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>60</v>
@@ -2515,16 +2539,20 @@
       <c r="E56" s="5">
         <v>42915</v>
       </c>
-      <c r="F56" s="4"/>
-      <c r="G56" s="5"/>
+      <c r="F56" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G56" s="7">
+        <v>44294</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B57" s="3"/>
-      <c r="C57" s="15" t="s">
-        <v>173</v>
+      <c r="C57" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>60</v>
@@ -2532,8 +2560,12 @@
       <c r="E57" s="5">
         <v>43228</v>
       </c>
-      <c r="F57" s="4"/>
-      <c r="G57" s="5"/>
+      <c r="F57" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="G57" s="7">
+        <v>44294</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
@@ -2541,7 +2573,7 @@
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>60</v>
@@ -2558,7 +2590,7 @@
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>60</v>
@@ -2575,12 +2607,18 @@
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="4" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="D60" s="4"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="3"/>
+      <c r="E60" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G60" s="7">
+        <v>42138</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
@@ -2588,14 +2626,20 @@
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F61" s="4"/>
-      <c r="G61" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61" s="5">
+        <v>42138</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G61" s="7">
+        <v>42139</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
@@ -2603,12 +2647,10 @@
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="4" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D62" s="4"/>
-      <c r="E62" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="E62" s="5"/>
       <c r="F62" s="4"/>
       <c r="G62" s="3"/>
     </row>
@@ -2618,18 +2660,14 @@
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="4" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F63" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G63" s="7">
-        <v>42138</v>
-      </c>
+      <c r="F63" s="4"/>
+      <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
@@ -2637,20 +2675,14 @@
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E64" s="5">
-        <v>42138</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G64" s="7">
-        <v>42139</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
@@ -2673,7 +2705,7 @@
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>60</v>
@@ -2690,7 +2722,7 @@
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>60</v>
@@ -2707,7 +2739,7 @@
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>60</v>
@@ -2724,7 +2756,7 @@
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="5" t="s">
@@ -2733,7 +2765,9 @@
       <c r="F69" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G69" s="3"/>
+      <c r="G69" s="7">
+        <v>42146</v>
+      </c>
     </row>
     <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
@@ -2741,18 +2775,16 @@
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G70" s="7">
-        <v>42146</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
@@ -2767,7 +2799,7 @@
         <v>38</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G71" s="3"/>
     </row>
@@ -2799,7 +2831,7 @@
         <v>38</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G73" s="3"/>
     </row>
@@ -2809,7 +2841,7 @@
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>60</v>
@@ -2826,7 +2858,7 @@
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>60</v>
@@ -2843,10 +2875,10 @@
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E76" s="5">
         <v>44041</v>
@@ -2860,7 +2892,7 @@
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>60</v>
@@ -2877,7 +2909,7 @@
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>60</v>
@@ -2903,7 +2935,7 @@
         <v>42066</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G79" s="7">
         <v>42146</v>
@@ -2924,7 +2956,7 @@
         <v>42023</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G80" s="7">
         <v>42146</v>
@@ -2936,14 +2968,14 @@
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G81" s="7">
         <v>42146</v>
@@ -2974,12 +3006,12 @@
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="5"/>
       <c r="F83" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G83" s="7">
         <v>42146</v>
@@ -2991,19 +3023,19 @@
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="4" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="E84" s="5">
-        <v>42188</v>
+        <v>42193</v>
       </c>
       <c r="F84" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G84" s="7">
-        <v>43194</v>
+        <v>42207</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3012,19 +3044,19 @@
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="E85" s="5">
-        <v>42193</v>
+        <v>42256</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G85" s="7">
-        <v>42207</v>
+        <v>42380</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3033,19 +3065,19 @@
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="4" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E86" s="5">
-        <v>42256</v>
+        <v>42188</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G86" s="7">
-        <v>42380</v>
+        <v>43194</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3054,7 +3086,7 @@
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>60</v>
@@ -3063,7 +3095,7 @@
         <v>42472</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G87" s="7"/>
     </row>
@@ -3073,7 +3105,7 @@
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>60</v>
@@ -3090,10 +3122,10 @@
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D89" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>190</v>
       </c>
       <c r="E89" s="5">
         <v>44084</v>
@@ -3103,11 +3135,11 @@
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>60</v>
@@ -3124,7 +3156,7 @@
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>50</v>
@@ -3192,10 +3224,10 @@
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D95" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="E95" s="5">
         <v>42205</v>
@@ -3213,19 +3245,19 @@
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E96" s="5">
         <v>42205</v>
       </c>
       <c r="F96" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G96" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -3234,10 +3266,10 @@
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="E97" s="5">
         <v>44278</v>
@@ -3245,131 +3277,156 @@
       <c r="F97" s="4"/>
       <c r="G97" s="3"/>
     </row>
+    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B98" s="3"/>
+      <c r="C98" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E98" s="5">
+        <v>44294</v>
+      </c>
+      <c r="F98" s="4"/>
+      <c r="G98" s="3"/>
+    </row>
   </sheetData>
   <autoFilter ref="A2:G96" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A79:H89">
+    <sortCondition ref="G79:G89"/>
+  </sortState>
   <conditionalFormatting sqref="C84:C87 C79:C82 C3:C13 C15 C54:C56 C31:C35 C68:C74 C22:C24 C90:C94 C20 C60:C66 C26 C28:C29 C37:C52">
-    <cfRule type="expression" dxfId="25" priority="34">
+    <cfRule type="expression" dxfId="26" priority="35">
       <formula>ISBLANK($G3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="expression" dxfId="24" priority="29">
+    <cfRule type="expression" dxfId="25" priority="30">
       <formula>ISBLANK($G76)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="expression" dxfId="23" priority="28">
+    <cfRule type="expression" dxfId="24" priority="29">
       <formula>ISBLANK($G83)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="expression" dxfId="22" priority="27">
+    <cfRule type="expression" dxfId="23" priority="28">
       <formula>ISBLANK($G95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C96">
-    <cfRule type="expression" dxfId="21" priority="26">
+    <cfRule type="expression" dxfId="22" priority="27">
       <formula>ISBLANK($G96)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="20" priority="25">
+    <cfRule type="expression" dxfId="21" priority="26">
       <formula>ISBLANK($G21)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="19" priority="24">
+    <cfRule type="expression" dxfId="20" priority="25">
       <formula>ISBLANK($G14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="18" priority="23">
+    <cfRule type="expression" dxfId="19" priority="24">
       <formula>ISBLANK($G53)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="17" priority="20">
+    <cfRule type="expression" dxfId="18" priority="21">
       <formula>ISBLANK($G67)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C89">
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>ISBLANK($G88)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>ISBLANK($G57)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>ISBLANK($G25)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>ISBLANK($G16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>ISBLANK($G17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>ISBLANK($G27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>ISBLANK($G18)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>ISBLANK($G36)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>ISBLANK($G78)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>ISBLANK($G77)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>ISBLANK($G58)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>ISBLANK($G19)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>ISBLANK($G30)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>ISBLANK($G75)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>ISBLANK($G59)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>ISBLANK($G97)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C98">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ISBLANK($G97)</formula>
+      <formula>ISBLANK($G98)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3400,67 +3457,67 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="M3" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q3" s="13" t="s">
         <v>162</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -3469,7 +3526,7 @@
       </c>
       <c r="C5" s="10"/>
       <c r="L5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -3478,36 +3535,36 @@
       </c>
       <c r="C6" s="12"/>
       <c r="P6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8" s="10">
         <v>42976</v>
       </c>
       <c r="C8" s="10"/>
       <c r="P8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9" s="10">
         <v>43017</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -3518,15 +3575,15 @@
         <v>43105</v>
       </c>
       <c r="P10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to network rank to accompany improvements to mvmeta, pbest. Corresponding additions to cscript.
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89769C03-01B9-4590-B16A-74E172A94879}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5717CA-E05D-495A-8F92-0984AB1C8B64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6390" yWindow="3630" windowWidth="10260" windowHeight="10005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="versions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$95</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'To do'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="221">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>NETWORK RANK</t>
-  </si>
-  <si>
-    <t>problems arising from pbest needing longparm:</t>
   </si>
   <si>
     <t>NETWORK SIDESPLIT</t>
@@ -750,6 +747,18 @@
   </si>
   <si>
     <t>as far as I can see, this is not a problem, but I've made metavars robust to model failing</t>
+  </si>
+  <si>
+    <t>used vwls</t>
+  </si>
+  <si>
+    <t>this was a mvmeta error but it's now ok as uses "`e(wscorr)'"</t>
+  </si>
+  <si>
+    <t>tough</t>
+  </si>
+  <si>
+    <t>added note</t>
   </si>
 </sst>
 </file>
@@ -908,12 +917,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1411,13 +1415,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F51" sqref="F51"/>
+      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,28 +1444,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1470,16 +1474,16 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="E3" s="5">
         <v>42045</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7">
         <v>42076</v>
@@ -1491,14 +1495,14 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" s="7">
         <v>42135</v>
@@ -1510,14 +1514,14 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" s="7">
         <v>42135</v>
@@ -1529,16 +1533,16 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="E6" s="5">
         <v>42157</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G6" s="7">
         <v>42163</v>
@@ -1550,16 +1554,16 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="5">
         <v>42191</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G7" s="7">
         <v>42191</v>
@@ -1571,16 +1575,16 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" s="5">
         <v>42191</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G8" s="7">
         <v>42191</v>
@@ -1592,16 +1596,16 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="5">
         <v>42314</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G9" s="7">
         <v>43194</v>
@@ -1613,16 +1617,16 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E10" s="5">
         <v>42388</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G10" s="7">
         <v>43194</v>
@@ -1634,16 +1638,16 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="5">
         <v>42166</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G11" s="7">
         <v>44293</v>
@@ -1655,16 +1659,16 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="5">
         <v>42242</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G12" s="7">
         <v>44293</v>
@@ -1676,16 +1680,16 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="5">
         <v>43250</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G13" s="7">
         <v>44293</v>
@@ -1697,22 +1701,22 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>175</v>
       </c>
       <c r="E14" s="5">
         <v>43085</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G14" s="7">
         <v>44293</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1721,22 +1725,22 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E15" s="18">
         <v>43593</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G15" s="7">
         <v>44293</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1745,16 +1749,16 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="18">
         <v>43712</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G16" s="7">
         <v>44293</v>
@@ -1766,17 +1770,17 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1785,16 +1789,16 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" s="5">
         <v>42166</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G18" s="7">
         <v>44294</v>
@@ -1806,16 +1810,16 @@
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="5">
         <v>42256</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G19" s="7"/>
     </row>
@@ -1825,16 +1829,16 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="5">
         <v>42045</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G20" s="7">
         <v>42135</v>
@@ -1846,16 +1850,16 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" s="5">
         <v>42045</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G21" s="7">
         <v>42135</v>
@@ -1871,10 +1875,10 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G22" s="7">
         <v>42135</v>
@@ -1886,22 +1890,22 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="E23" s="5">
         <v>42262</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G23" s="7">
         <v>44293</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1910,16 +1914,16 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="5">
         <v>43238</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G24" s="7">
         <v>44293</v>
@@ -1931,16 +1935,16 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="5">
         <v>43356</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G25" s="7">
         <v>44293</v>
@@ -1952,22 +1956,22 @@
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E26" s="18">
         <v>43593</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G26" s="7">
         <v>44293</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1976,10 +1980,10 @@
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E27" s="5">
         <v>42045</v>
@@ -1998,10 +2002,10 @@
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G28" s="8">
         <v>42077</v>
@@ -2013,16 +2017,16 @@
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E29" s="5">
         <v>42314</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G29" s="8">
         <v>42964</v>
@@ -2034,16 +2038,16 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E30" s="5">
         <v>43017</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G30" s="8">
         <v>43712</v>
@@ -2070,10 +2074,10 @@
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="G32" s="7">
         <v>42135</v>
@@ -2085,16 +2089,16 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E33" s="5">
         <v>42137</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G33" s="7">
         <v>42139</v>
@@ -2106,16 +2110,16 @@
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E34" s="5">
         <v>42137</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G34" s="7">
         <v>44293</v>
@@ -2127,16 +2131,16 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="E35" s="5">
         <v>41914</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G35" s="19">
         <v>44294</v>
@@ -2148,22 +2152,22 @@
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E36" s="18">
         <v>43593</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G36" s="19">
         <v>44294</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2205,14 +2209,14 @@
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G40" s="7">
         <v>42137</v>
@@ -2224,14 +2228,14 @@
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="5">
         <v>42135</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G41" s="7">
         <v>42137</v>
@@ -2243,16 +2247,16 @@
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="E42" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G42" s="7">
         <v>42137</v>
@@ -2264,16 +2268,16 @@
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E43" s="5">
         <v>42137</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G43" s="7">
         <v>42137</v>
@@ -2285,12 +2289,12 @@
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="5"/>
       <c r="F44" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G44" s="7">
         <v>42138</v>
@@ -2302,16 +2306,16 @@
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="E45" s="5">
         <v>41934</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G45" s="7">
         <v>42138</v>
@@ -2323,16 +2327,16 @@
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E46" s="5">
         <v>41934</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G46" s="7">
         <v>42138</v>
@@ -2344,16 +2348,16 @@
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E47" s="5">
         <v>42137</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G47" s="7">
         <v>42138</v>
@@ -2365,16 +2369,16 @@
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E48" s="5">
         <v>42915</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G48" s="5">
         <v>42915</v>
@@ -2386,16 +2390,16 @@
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E49" s="5">
         <v>42619</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G49" s="7">
         <v>43194</v>
@@ -2411,10 +2415,10 @@
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G50" s="7">
         <v>44294</v>
@@ -2429,13 +2433,13 @@
         <v>14</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G51" s="7">
         <v>44294</v>
@@ -2447,16 +2451,16 @@
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="E52" s="5">
         <v>42176</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G52" s="7">
         <v>44294</v>
@@ -2468,16 +2472,16 @@
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E53" s="5">
         <v>42179</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G53" s="7">
         <v>44294</v>
@@ -2489,16 +2493,16 @@
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E54" s="5">
         <v>42242</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G54" s="7">
         <v>44294</v>
@@ -2510,16 +2514,16 @@
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E55" s="5">
         <v>42348</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G55" s="7">
         <v>44294</v>
@@ -2531,16 +2535,16 @@
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E56" s="5">
         <v>42915</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G56" s="7">
         <v>44294</v>
@@ -2552,16 +2556,16 @@
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E57" s="5">
         <v>43228</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G57" s="7">
         <v>44294</v>
@@ -2573,33 +2577,41 @@
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E58" s="5">
         <v>43672</v>
       </c>
-      <c r="F58" s="4"/>
-      <c r="G58" s="5"/>
-    </row>
-    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F58" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G58" s="7">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E59" s="5">
         <v>44144</v>
       </c>
-      <c r="F59" s="4"/>
-      <c r="G59" s="5"/>
+      <c r="F59" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="G59" s="7">
+        <v>44294</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
@@ -2607,14 +2619,14 @@
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G60" s="7">
         <v>42138</v>
@@ -2626,16 +2638,16 @@
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E61" s="5">
         <v>42138</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G61" s="7">
         <v>42139</v>
@@ -2647,12 +2659,18 @@
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="4" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D62" s="4"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="3"/>
+      <c r="E62" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="G62" s="7">
+        <v>44294</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
@@ -2664,25 +2682,33 @@
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F63" s="4"/>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="G63" s="7">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="4" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="D64" s="4"/>
-      <c r="E64" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F64" s="4"/>
-      <c r="G64" s="3"/>
+      <c r="E64" s="5">
+        <v>42137</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G64" s="7">
+        <v>44294</v>
+      </c>
     </row>
     <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
@@ -2690,31 +2716,41 @@
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D65" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="E65" s="5">
-        <v>42137</v>
-      </c>
-      <c r="F65" s="4"/>
-      <c r="G65" s="3"/>
-    </row>
-    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42138</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G65" s="7">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="4" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E66" s="5">
-        <v>42138</v>
-      </c>
-      <c r="F66" s="4"/>
-      <c r="G66" s="3"/>
+        <v>42348</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G66" s="7">
+        <v>44294</v>
+      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
@@ -2722,90 +2758,92 @@
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="4" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E67" s="5">
-        <v>42348</v>
-      </c>
-      <c r="F67" s="4"/>
-      <c r="G67" s="3"/>
+        <v>43017</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G67" s="7">
+        <v>44294</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E68" s="5">
-        <v>43017</v>
-      </c>
-      <c r="F68" s="4"/>
-      <c r="G68" s="3"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G68" s="7">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G69" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F71" s="4"/>
       <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="4" t="s">
@@ -2813,89 +2851,91 @@
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F72" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="G72" s="3"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D73" s="4"/>
-      <c r="E73" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>87</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E73" s="5">
+        <v>42146</v>
+      </c>
+      <c r="F73" s="4"/>
       <c r="G73" s="3"/>
     </row>
-    <row r="74" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="4" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E74" s="5">
-        <v>42146</v>
+        <v>42163</v>
       </c>
       <c r="F74" s="4"/>
       <c r="G74" s="3"/>
     </row>
     <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="4" t="s">
-        <v>97</v>
+        <v>186</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>60</v>
+        <v>185</v>
       </c>
       <c r="E75" s="5">
-        <v>42163</v>
+        <v>44041</v>
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="3"/>
     </row>
-    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>186</v>
+        <v>59</v>
       </c>
       <c r="E76" s="5">
-        <v>44041</v>
+        <v>43672</v>
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="3"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="4" t="s">
         <v>180</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E77" s="5">
         <v>43672</v>
@@ -2903,464 +2943,447 @@
       <c r="F77" s="4"/>
       <c r="G77" s="3"/>
     </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="4" t="s">
-        <v>181</v>
+        <v>48</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E78" s="5">
-        <v>43672</v>
-      </c>
-      <c r="F78" s="4"/>
-      <c r="G78" s="3"/>
-    </row>
-    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>42066</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G78" s="7">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E79" s="5">
-        <v>42066</v>
+        <v>42023</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G79" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E80" s="5">
-        <v>42023</v>
+        <v>79</v>
+      </c>
+      <c r="D80" s="4"/>
+      <c r="E80" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G80" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="4" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="G81" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="4" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="D82" s="4"/>
-      <c r="E82" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="E82" s="5"/>
       <c r="F82" s="4" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="G82" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D83" s="4"/>
-      <c r="E83" s="5"/>
+        <v>108</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E83" s="5">
+        <v>42193</v>
+      </c>
       <c r="F83" s="4" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="G83" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="4" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="E84" s="5">
-        <v>42193</v>
+        <v>42256</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G84" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>42380</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="4" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E85" s="5">
-        <v>42256</v>
+        <v>42188</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G85" s="7">
-        <v>42380</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="4" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E86" s="5">
-        <v>42188</v>
+        <v>42472</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G86" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="G86" s="7"/>
+    </row>
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="4" t="s">
-        <v>128</v>
+        <v>169</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E87" s="5">
-        <v>42472</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>169</v>
-      </c>
+        <v>43238</v>
+      </c>
+      <c r="F87" s="4"/>
       <c r="G87" s="7"/>
     </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="4" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>60</v>
+        <v>188</v>
       </c>
       <c r="E88" s="5">
-        <v>43238</v>
+        <v>44084</v>
       </c>
       <c r="F88" s="4"/>
       <c r="G88" s="7"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B89" s="3"/>
+      <c r="C89" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E89" s="5">
+        <v>44214</v>
+      </c>
+      <c r="F89" s="4"/>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B89" s="3"/>
-      <c r="C89" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="E89" s="5">
-        <v>44084</v>
-      </c>
-      <c r="F89" s="4"/>
-      <c r="G89" s="7"/>
-    </row>
-    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="B90" s="3"/>
-      <c r="C90" s="21" t="s">
-        <v>192</v>
+      <c r="C90" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E90" s="5">
-        <v>44214</v>
+        <v>42157</v>
       </c>
       <c r="F90" s="4"/>
       <c r="G90" s="3"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E91" s="5">
-        <v>42157</v>
+        <v>23</v>
+      </c>
+      <c r="D91" s="4"/>
+      <c r="E91" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F91" s="4"/>
       <c r="G91" s="3"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F92" s="4"/>
-      <c r="G92" s="3"/>
-    </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G92" s="7">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D93" s="4"/>
-      <c r="E93" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G93" s="7">
-        <v>43194</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E93" s="5">
+        <v>42135</v>
+      </c>
+      <c r="F93" s="4"/>
+      <c r="G93" s="3"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="4" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="E94" s="5">
-        <v>42135</v>
-      </c>
-      <c r="F94" s="4"/>
-      <c r="G94" s="3"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42205</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G94" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D95" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="E95" s="5">
         <v>42205</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G95" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="4" t="s">
-        <v>129</v>
+        <v>192</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>112</v>
+        <v>193</v>
       </c>
       <c r="E96" s="5">
-        <v>42205</v>
-      </c>
-      <c r="F96" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44278</v>
+      </c>
+      <c r="F96" s="4"/>
+      <c r="G96" s="3"/>
+    </row>
+    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="4" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>194</v>
+        <v>59</v>
       </c>
       <c r="E97" s="5">
-        <v>44278</v>
+        <v>44294</v>
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="3"/>
     </row>
-    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E98" s="5">
-        <v>44294</v>
-      </c>
-      <c r="F98" s="4"/>
-      <c r="G98" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:G96" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A79:H89">
-    <sortCondition ref="G79:G89"/>
+  <autoFilter ref="A2:G95" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A78:H88">
+    <sortCondition ref="G78:G88"/>
   </sortState>
-  <conditionalFormatting sqref="C84:C87 C79:C82 C3:C13 C15 C54:C56 C31:C35 C68:C74 C22:C24 C90:C94 C20 C60:C66 C26 C28:C29 C37:C52">
-    <cfRule type="expression" dxfId="26" priority="35">
+  <conditionalFormatting sqref="C83:C86 C78:C81 C3:C13 C15 C54:C56 C31:C35 C67:C73 C22:C24 C89:C93 C20 C26 C28:C29 C37:C52 C60:C65">
+    <cfRule type="expression" dxfId="25" priority="35">
       <formula>ISBLANK($G3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
-    <cfRule type="expression" dxfId="25" priority="30">
-      <formula>ISBLANK($G76)</formula>
+  <conditionalFormatting sqref="C75">
+    <cfRule type="expression" dxfId="24" priority="30">
+      <formula>ISBLANK($G75)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C83">
-    <cfRule type="expression" dxfId="24" priority="29">
-      <formula>ISBLANK($G83)</formula>
+  <conditionalFormatting sqref="C82">
+    <cfRule type="expression" dxfId="23" priority="29">
+      <formula>ISBLANK($G82)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C94">
+    <cfRule type="expression" dxfId="22" priority="28">
+      <formula>ISBLANK($G94)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="expression" dxfId="23" priority="28">
+    <cfRule type="expression" dxfId="21" priority="27">
       <formula>ISBLANK($G95)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C96">
-    <cfRule type="expression" dxfId="22" priority="27">
-      <formula>ISBLANK($G96)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="21" priority="26">
+    <cfRule type="expression" dxfId="20" priority="26">
       <formula>ISBLANK($G21)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="20" priority="25">
+    <cfRule type="expression" dxfId="19" priority="25">
       <formula>ISBLANK($G14)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="19" priority="24">
+    <cfRule type="expression" dxfId="18" priority="24">
       <formula>ISBLANK($G53)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="18" priority="21">
-      <formula>ISBLANK($G67)</formula>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" dxfId="17" priority="21">
+      <formula>ISBLANK($G66)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C88:C89">
-    <cfRule type="expression" dxfId="17" priority="19">
-      <formula>ISBLANK($G88)</formula>
+  <conditionalFormatting sqref="C87:C88">
+    <cfRule type="expression" dxfId="16" priority="19">
+      <formula>ISBLANK($G87)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="15" priority="17">
       <formula>ISBLANK($G57)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>ISBLANK($G25)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>ISBLANK($G16)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3384,14 +3407,14 @@
       <formula>ISBLANK($G36)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C78">
+  <conditionalFormatting sqref="C77">
     <cfRule type="expression" dxfId="8" priority="9">
-      <formula>ISBLANK($G78)</formula>
+      <formula>ISBLANK($G77)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
+  <conditionalFormatting sqref="C76">
     <cfRule type="expression" dxfId="7" priority="8">
-      <formula>ISBLANK($G77)</formula>
+      <formula>ISBLANK($G76)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
@@ -3409,9 +3432,9 @@
       <formula>ISBLANK($G30)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C75">
+  <conditionalFormatting sqref="C74">
     <cfRule type="expression" dxfId="3" priority="4">
-      <formula>ISBLANK($G75)</formula>
+      <formula>ISBLANK($G74)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
@@ -3419,14 +3442,14 @@
       <formula>ISBLANK($G59)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C97">
+  <conditionalFormatting sqref="C96">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>ISBLANK($G97)</formula>
+      <formula>ISBLANK($G96)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C98">
+  <conditionalFormatting sqref="C97">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ISBLANK($G98)</formula>
+      <formula>ISBLANK($G97)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3457,67 +3480,67 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="M3" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q3" s="13" t="s">
         <v>161</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -3526,7 +3549,7 @@
       </c>
       <c r="C5" s="10"/>
       <c r="L5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -3535,36 +3558,36 @@
       </c>
       <c r="C6" s="12"/>
       <c r="P6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B8" s="10">
         <v>42976</v>
       </c>
       <c r="C8" s="10"/>
       <c r="P8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B9" s="10">
         <v>43017</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -3575,15 +3598,15 @@
         <v>43105</v>
       </c>
       <c r="P10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve error handling for treatment names with network setup, nocodes
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72991787-2ED7-422C-9D7A-557CDD672C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16462B8-64B0-4469-90E2-B7621AA8EF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1008" yWindow="792" windowWidth="16656" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="4512" windowWidth="16656" windowHeight="12168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To do" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="231">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -764,9 +764,6 @@
     <t>me/Katharine Nix</t>
   </si>
   <si>
-    <t>trim blanks from treatment names</t>
-  </si>
-  <si>
     <t>remove version numbers from sub-files, they are confusing</t>
   </si>
   <si>
@@ -777,6 +774,21 @@
   </si>
   <si>
     <t>update FAQs</t>
+  </si>
+  <si>
+    <t>enable component NMA?</t>
+  </si>
+  <si>
+    <t>network rank?</t>
+  </si>
+  <si>
+    <t>better error if sencode is not installed</t>
+  </si>
+  <si>
+    <t>done, and give better error when non-alphanumeric characeters used</t>
+  </si>
+  <si>
+    <t>trim blanks from treatment names with nocodes option</t>
   </si>
 </sst>
 </file>
@@ -1445,10 +1457,10 @@
   <dimension ref="A1:H105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1850,13 +1862,13 @@
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>221</v>
@@ -1864,8 +1876,12 @@
       <c r="E20" s="5">
         <v>44312</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="7"/>
+      <c r="F20" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G20" s="7">
+        <v>44434</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -3206,7 +3222,7 @@
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>59</v>
@@ -3215,7 +3231,7 @@
         <v>44214</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G90" s="7">
         <v>44434</v>
@@ -3375,7 +3391,7 @@
       </c>
       <c r="B99" s="3"/>
       <c r="C99" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>59</v>
@@ -3392,7 +3408,7 @@
       </c>
       <c r="B100" s="3"/>
       <c r="C100" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>59</v>
@@ -3404,20 +3420,36 @@
       <c r="G100" s="3"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" s="3"/>
+      <c r="A101" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B101" s="3"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-      <c r="E101" s="5"/>
+      <c r="C101" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E101" s="5">
+        <v>44434</v>
+      </c>
       <c r="F101" s="4"/>
       <c r="G101" s="3"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A102" s="3"/>
+      <c r="A102" s="3" t="s">
+        <v>227</v>
+      </c>
       <c r="B102" s="3"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
-      <c r="E102" s="5"/>
+      <c r="C102" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E102" s="5">
+        <v>44312</v>
+      </c>
       <c r="F102" s="4"/>
       <c r="G102" s="3"/>
     </row>

</xml_diff>

<commit_message>
Improve format of network.sthlp
</commit_message>
<xml_diff>
--- a/network-to-do.xlsx
+++ b/network-to-do.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ado\ian\network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185DE178-36B2-41FB-B5CB-45CBAAD7D42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B04293C-DFE1-4BD1-8826-B9ACC1F7CC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12015" yWindow="3450" windowWidth="23010" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To do" sheetId="1" r:id="rId1"/>
     <sheet name="versions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do'!$A$2:$G$97</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'To do'!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -65,7 +65,7 @@
     need to print a warning that network meta will fail (but network map may succeed)</t>
       </text>
     </comment>
-    <comment ref="C59" authorId="2" shapeId="0" xr:uid="{ED6B4446-BECB-4AC2-AC74-C14778DF40D1}">
+    <comment ref="C60" authorId="2" shapeId="0" xr:uid="{ED6B4446-BECB-4AC2-AC74-C14778DF40D1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -74,7 +74,7 @@
 reg _y _trtdiff_C _trtdiff_D [aw=1/_stderr^2], mse1 noconstant</t>
       </text>
     </comment>
-    <comment ref="C60" authorId="3" shapeId="0" xr:uid="{50F99A35-5AC1-458D-8F00-D63EFAC00865}">
+    <comment ref="C61" authorId="3" shapeId="0" xr:uid="{50F99A35-5AC1-458D-8F00-D63EFAC00865}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="233">
   <si>
     <t>TO-DO LIST FOR NETWORK</t>
   </si>
@@ -792,6 +792,9 @@
   </si>
   <si>
     <t>written - still to test fully</t>
+  </si>
+  <si>
+    <t>compute df from design variable</t>
   </si>
 </sst>
 </file>
@@ -932,7 +935,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1429,11 +1437,11 @@
   <threadedComment ref="C26" personId="{5D58C562-25D2-4493-B339-1D5F20B1863B}" id="{EBD4C436-E631-4AF3-8DA4-6B56C6A448C0}">
     <text>need to print a warning that network meta will fail (but network map may succeed)</text>
   </threadedComment>
-  <threadedComment ref="C59" personId="{5D58C562-25D2-4493-B339-1D5F20B1863B}" id="{ED6B4446-BECB-4AC2-AC74-C14778DF40D1}">
+  <threadedComment ref="C60" personId="{5D58C562-25D2-4493-B339-1D5F20B1863B}" id="{ED6B4446-BECB-4AC2-AC74-C14778DF40D1}">
     <text>e.g.
 reg _y _trtdiff_C _trtdiff_D [aw=1/_stderr^2], mse1 noconstant</text>
   </threadedComment>
-  <threadedComment ref="C60" personId="{5D58C562-25D2-4493-B339-1D5F20B1863B}" id="{50F99A35-5AC1-458D-8F00-D63EFAC00865}">
+  <threadedComment ref="C61" personId="{5D58C562-25D2-4493-B339-1D5F20B1863B}" id="{50F99A35-5AC1-458D-8F00-D63EFAC00865}">
     <text>e.g.
 reg _y _trtdiff_C _trtdiff_D [aw=1/_stderr^2], mse1 noconstant</text>
   </threadedComment>
@@ -1445,13 +1453,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,125 +2057,122 @@
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="7">
-        <v>42077</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="5">
+        <v>44449</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="5">
-        <v>42314</v>
+        <v>5</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="G30" s="7">
-        <v>42964</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42077</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="15" t="s">
-        <v>144</v>
+      <c r="C31" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E31" s="5">
-        <v>43017</v>
+        <v>42314</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="G31" s="7">
-        <v>43712</v>
+        <v>42964</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="3"/>
+      <c r="C32" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="5">
+        <v>43017</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G32" s="7">
+        <v>43712</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" s="3"/>
-      <c r="C33" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="7">
-        <v>42135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="E33" s="5"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="5">
-        <v>42137</v>
+        <v>8</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="G34" s="7">
-        <v>42139</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>42135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="4" t="s">
-        <v>208</v>
+        <v>72</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>59</v>
@@ -2176,31 +2181,31 @@
         <v>42137</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>209</v>
+        <v>83</v>
       </c>
       <c r="G35" s="7">
-        <v>44293</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>42139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="4" t="s">
-        <v>43</v>
+        <v>208</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="E36" s="5">
-        <v>41914</v>
+        <v>42137</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="G36" s="17">
-        <v>44294</v>
+        <v>209</v>
+      </c>
+      <c r="G36" s="7">
+        <v>44293</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2209,38 +2214,48 @@
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="E37" s="16">
-        <v>43593</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>205</v>
+        <v>43</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="5">
+        <v>41914</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="G37" s="17">
         <v>44294</v>
       </c>
-      <c r="H37" s="1" t="s">
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" s="16">
+        <v>43593</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="G38" s="17">
+        <v>44294</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
@@ -2251,7 +2266,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
@@ -2262,117 +2277,107 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41" s="3"/>
-      <c r="C41" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G41" s="7">
-        <v>42137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="E41" s="5"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="4" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D42" s="4"/>
-      <c r="E42" s="5">
-        <v>42135</v>
+      <c r="E42" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G42" s="7">
         <v>42137</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>37</v>
+        <v>60</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="5">
+        <v>42135</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G43" s="7">
         <v>42137</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E44" s="5">
-        <v>42137</v>
+        <v>63</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G44" s="7">
         <v>42137</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="5">
+        <v>42137</v>
+      </c>
       <c r="F45" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G45" s="7">
-        <v>42138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>42137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E46" s="5">
-        <v>41934</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="5"/>
       <c r="F46" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G46" s="7">
         <v>42138</v>
@@ -2384,7 +2389,7 @@
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>46</v>
@@ -2405,16 +2410,16 @@
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="4" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E48" s="5">
-        <v>42137</v>
+        <v>41934</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G48" s="7">
         <v>42138</v>
@@ -2426,19 +2431,19 @@
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="4" t="s">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E49" s="5">
-        <v>42915</v>
+        <v>42137</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="G49" s="5">
-        <v>42915</v>
+        <v>76</v>
+      </c>
+      <c r="G49" s="7">
+        <v>42138</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2447,56 +2452,56 @@
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E50" s="5">
-        <v>42619</v>
+        <v>42915</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="G50" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="G50" s="5">
+        <v>42915</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="5" t="s">
-        <v>37</v>
+        <v>129</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E51" s="5">
+        <v>42619</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>215</v>
+        <v>149</v>
       </c>
       <c r="G51" s="7">
-        <v>44294</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>59</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D52" s="4"/>
       <c r="E52" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="G52" s="7">
         <v>44294</v>
@@ -2508,13 +2513,13 @@
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="4" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E53" s="5">
-        <v>42176</v>
+        <v>59</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>207</v>
@@ -2523,43 +2528,43 @@
         <v>44294</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="E54" s="5">
-        <v>42179</v>
+        <v>42176</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>86</v>
+        <v>207</v>
       </c>
       <c r="G54" s="7">
         <v>44294</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="4" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="E55" s="5">
-        <v>42242</v>
+        <v>42179</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>210</v>
+        <v>86</v>
       </c>
       <c r="G55" s="7">
         <v>44294</v>
@@ -2571,58 +2576,58 @@
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="E56" s="5">
-        <v>42348</v>
+        <v>42242</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G56" s="7">
         <v>44294</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="4" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E57" s="5">
-        <v>42915</v>
+        <v>42348</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G57" s="7">
         <v>44294</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B58" s="3"/>
-      <c r="C58" s="15" t="s">
-        <v>171</v>
+      <c r="C58" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E58" s="5">
-        <v>43228</v>
+        <v>42915</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G58" s="7">
         <v>44294</v>
@@ -2634,59 +2639,61 @@
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="15" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E59" s="5">
-        <v>43672</v>
+        <v>43228</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G59" s="7">
         <v>44294</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="15" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E60" s="5">
-        <v>44144</v>
+        <v>43672</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G60" s="7">
         <v>44294</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B61" s="3"/>
-      <c r="C61" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="5" t="s">
-        <v>37</v>
+      <c r="C61" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E61" s="5">
+        <v>44144</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>66</v>
+        <v>217</v>
       </c>
       <c r="G61" s="7">
-        <v>42138</v>
+        <v>44294</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2695,19 +2702,17 @@
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E62" s="5">
+        <v>52</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G62" s="7">
         <v>42138</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G62" s="7">
-        <v>42139</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2716,17 +2721,19 @@
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D63" s="4"/>
-      <c r="E63" s="5" t="s">
-        <v>37</v>
+        <v>81</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E63" s="5">
+        <v>42138</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>218</v>
+        <v>84</v>
       </c>
       <c r="G63" s="7">
-        <v>44294</v>
+        <v>42139</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2735,7 +2742,7 @@
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="5" t="s">
@@ -2748,20 +2755,20 @@
         <v>44294</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="4" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="D65" s="4"/>
-      <c r="E65" s="5">
-        <v>42137</v>
+      <c r="E65" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G65" s="7">
         <v>44294</v>
@@ -2773,34 +2780,32 @@
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>59</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D66" s="4"/>
       <c r="E66" s="5">
-        <v>42138</v>
+        <v>42137</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="G66" s="7">
         <v>44294</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="4" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E67" s="5">
-        <v>42348</v>
+        <v>42138</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>183</v>
@@ -2815,56 +2820,60 @@
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="4" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E68" s="5">
-        <v>43017</v>
+        <v>42348</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>66</v>
+        <v>183</v>
       </c>
       <c r="G68" s="7">
         <v>44294</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D69" s="4"/>
-      <c r="E69" s="5" t="s">
-        <v>37</v>
+        <v>145</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E69" s="5">
+        <v>43017</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="G69" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G70" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="G70" s="7">
+        <v>42146</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
@@ -2872,14 +2881,14 @@
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="4" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G71" s="3"/>
     </row>
@@ -2889,13 +2898,15 @@
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="4" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F72" s="4"/>
+      <c r="F72" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2904,47 +2915,45 @@
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F73" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="F73" s="4"/>
       <c r="G73" s="3"/>
     </row>
-    <row r="74" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E74" s="5">
-        <v>42146</v>
-      </c>
-      <c r="F74" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D74" s="4"/>
+      <c r="E74" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="G74" s="3"/>
     </row>
-    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="4" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E75" s="5">
-        <v>42163</v>
+        <v>42146</v>
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="3"/>
@@ -2955,41 +2964,41 @@
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
-        <v>186</v>
+        <v>96</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>185</v>
+        <v>59</v>
       </c>
       <c r="E76" s="5">
-        <v>44041</v>
+        <v>42163</v>
       </c>
       <c r="F76" s="4"/>
       <c r="G76" s="3"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="4" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>59</v>
+        <v>185</v>
       </c>
       <c r="E77" s="5">
-        <v>43672</v>
+        <v>44041</v>
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="3"/>
     </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>59</v>
@@ -3000,98 +3009,98 @@
       <c r="F78" s="4"/>
       <c r="G78" s="3"/>
     </row>
-    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="4" t="s">
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E79" s="5">
-        <v>42066</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G79" s="7">
-        <v>42146</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>43672</v>
+      </c>
+      <c r="F79" s="4"/>
+      <c r="G79" s="3"/>
+    </row>
+    <row r="80" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E80" s="5">
-        <v>42023</v>
+        <v>42066</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G80" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D81" s="4"/>
-      <c r="E81" s="5" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E81" s="5">
+        <v>42023</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G81" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="4" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="G82" s="7">
         <v>42146</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="4" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="D83" s="4"/>
-      <c r="E83" s="5"/>
+      <c r="E83" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F83" s="4" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="G83" s="7">
         <v>42146</v>
@@ -3103,40 +3112,36 @@
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E84" s="5">
-        <v>42193</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D84" s="4"/>
+      <c r="E84" s="5"/>
       <c r="F84" s="4" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="G84" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="E85" s="5">
-        <v>42256</v>
+        <v>42193</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>66</v>
       </c>
       <c r="G85" s="7">
-        <v>42380</v>
+        <v>42207</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3145,111 +3150,115 @@
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="4" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E86" s="5">
-        <v>42188</v>
+        <v>42256</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>66</v>
       </c>
       <c r="G86" s="7">
-        <v>43194</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>42380</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="4" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E87" s="5">
-        <v>42472</v>
+        <v>42188</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="G87" s="7"/>
-    </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G87" s="7">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="4" t="s">
-        <v>169</v>
+        <v>127</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E88" s="5">
-        <v>43238</v>
-      </c>
-      <c r="F88" s="4"/>
+        <v>42472</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>168</v>
+      </c>
       <c r="G88" s="7"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="4" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>188</v>
+        <v>59</v>
       </c>
       <c r="E89" s="5">
-        <v>44084</v>
+        <v>43238</v>
       </c>
       <c r="F89" s="4"/>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="C90" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E90" s="5">
+        <v>44084</v>
+      </c>
+      <c r="F90" s="4"/>
+      <c r="G90" s="7"/>
+    </row>
+    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B90" s="3"/>
-      <c r="C90" s="19" t="s">
+      <c r="B91" s="3"/>
+      <c r="C91" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="D90" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E90" s="5">
+      <c r="D91" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E91" s="5">
         <v>44214</v>
       </c>
-      <c r="F90" s="4" t="s">
+      <c r="F91" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="G90" s="7">
+      <c r="G91" s="7">
         <v>44434</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B91" s="3"/>
-      <c r="C91" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E91" s="5">
-        <v>42157</v>
-      </c>
-      <c r="F91" s="4"/>
-      <c r="G91" s="3"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
@@ -3257,83 +3266,79 @@
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D92" s="4"/>
-      <c r="E92" s="5" t="s">
-        <v>37</v>
+        <v>95</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E92" s="5">
+        <v>42157</v>
       </c>
       <c r="F92" s="4"/>
       <c r="G92" s="3"/>
     </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F93" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G93" s="7">
-        <v>43194</v>
-      </c>
+      <c r="F93" s="4"/>
+      <c r="G93" s="3"/>
     </row>
     <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E94" s="5">
-        <v>42135</v>
+        <v>25</v>
+      </c>
+      <c r="D94" s="4"/>
+      <c r="E94" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>220</v>
+        <v>66</v>
       </c>
       <c r="G94" s="7">
-        <v>44294</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43194</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="4" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="E95" s="5">
-        <v>42205</v>
+        <v>42135</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>66</v>
+        <v>220</v>
       </c>
       <c r="G95" s="7">
-        <v>42207</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="4" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>111</v>
@@ -3342,59 +3347,63 @@
         <v>42205</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="G96" s="7">
+        <v>42207</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="4" t="s">
-        <v>191</v>
+        <v>128</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>192</v>
+        <v>111</v>
       </c>
       <c r="E97" s="5">
-        <v>44278</v>
-      </c>
-      <c r="F97" s="4"/>
-      <c r="G97" s="3"/>
-    </row>
-    <row r="98" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42205</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="4" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>59</v>
+        <v>192</v>
       </c>
       <c r="E98" s="5">
-        <v>44294</v>
+        <v>44278</v>
       </c>
       <c r="F98" s="4"/>
       <c r="G98" s="3"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B99" s="3"/>
       <c r="C99" s="4" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E99" s="5">
-        <v>44434</v>
+        <v>44294</v>
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="3"/>
@@ -3405,7 +3414,7 @@
       </c>
       <c r="B100" s="3"/>
       <c r="C100" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>59</v>
@@ -3418,11 +3427,11 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>59</v>
@@ -3433,29 +3442,37 @@
       <c r="F101" s="4"/>
       <c r="G101" s="3"/>
     </row>
-    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>227</v>
+        <v>12</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>221</v>
+        <v>59</v>
       </c>
       <c r="E102" s="5">
-        <v>44312</v>
+        <v>44434</v>
       </c>
       <c r="F102" s="4"/>
       <c r="G102" s="3"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="3"/>
+    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>227</v>
+      </c>
       <c r="B103" s="3"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="5"/>
+      <c r="C103" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E103" s="5">
+        <v>44312</v>
+      </c>
       <c r="F103" s="4"/>
       <c r="G103" s="3"/>
     </row>
@@ -3477,94 +3494,108 @@
       <c r="F105" s="4"/>
       <c r="G105" s="3"/>
     </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:G96" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A79:H89">
-    <sortCondition ref="G79:G89"/>
+  <autoFilter ref="A2:G97" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A80:H90">
+    <sortCondition ref="G80:G90"/>
   </sortState>
-  <conditionalFormatting sqref="C84:C87 C79:C82 C3:C13 C15 C55:C57 C32:C36 C68:C74 C23:C25 C90:C94 C21 C27 C29:C30 C38:C53 C61:C66">
-    <cfRule type="expression" dxfId="28" priority="38">
+  <conditionalFormatting sqref="C85:C88 C80:C83 C3:C13 C15 C56:C58 C33:C37 C69:C75 C23:C25 C91:C95 C21 C27 C30:C31 C39:C54 C62:C67">
+    <cfRule type="expression" dxfId="29" priority="39">
       <formula>ISBLANK($G3)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
-    <cfRule type="expression" dxfId="27" priority="33">
-      <formula>ISBLANK($G76)</formula>
+  <conditionalFormatting sqref="C77">
+    <cfRule type="expression" dxfId="28" priority="34">
+      <formula>ISBLANK($G77)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C83">
-    <cfRule type="expression" dxfId="26" priority="32">
-      <formula>ISBLANK($G83)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C95">
-    <cfRule type="expression" dxfId="25" priority="31">
-      <formula>ISBLANK($G95)</formula>
+  <conditionalFormatting sqref="C84">
+    <cfRule type="expression" dxfId="27" priority="33">
+      <formula>ISBLANK($G84)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C96">
-    <cfRule type="expression" dxfId="24" priority="30">
+    <cfRule type="expression" dxfId="26" priority="32">
       <formula>ISBLANK($G96)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C97">
+    <cfRule type="expression" dxfId="25" priority="31">
+      <formula>ISBLANK($G97)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="23" priority="29">
+    <cfRule type="expression" dxfId="24" priority="30">
       <formula>ISBLANK($G22)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="22" priority="28">
+    <cfRule type="expression" dxfId="23" priority="29">
       <formula>ISBLANK($G14)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="21" priority="27">
-      <formula>ISBLANK($G54)</formula>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="expression" dxfId="22" priority="28">
+      <formula>ISBLANK($G55)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="20" priority="24">
-      <formula>ISBLANK($G67)</formula>
+  <conditionalFormatting sqref="C68">
+    <cfRule type="expression" dxfId="21" priority="25">
+      <formula>ISBLANK($G68)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C88:C89">
-    <cfRule type="expression" dxfId="19" priority="22">
-      <formula>ISBLANK($G88)</formula>
+  <conditionalFormatting sqref="C89:C90">
+    <cfRule type="expression" dxfId="20" priority="23">
+      <formula>ISBLANK($G89)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="18" priority="20">
-      <formula>ISBLANK($G58)</formula>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>ISBLANK($G59)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="18" priority="20">
       <formula>ISBLANK($G26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>ISBLANK($G16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>ISBLANK($G17)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>ISBLANK($G28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>ISBLANK($G18)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C38">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>ISBLANK($G38)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C79">
     <cfRule type="expression" dxfId="12" priority="13">
-      <formula>ISBLANK($G37)</formula>
+      <formula>ISBLANK($G79)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78">
@@ -3572,59 +3603,59 @@
       <formula>ISBLANK($G78)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
+  <conditionalFormatting sqref="C60">
     <cfRule type="expression" dxfId="10" priority="11">
-      <formula>ISBLANK($G77)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>ISBLANK($G59)</formula>
+      <formula>ISBLANK($G60)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>ISBLANK($G19)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>ISBLANK($G31)</formula>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>ISBLANK($G32)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C75">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>ISBLANK($G75)</formula>
+  <conditionalFormatting sqref="C76">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>ISBLANK($G76)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>ISBLANK($G60)</formula>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>ISBLANK($G61)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C97">
+  <conditionalFormatting sqref="C98">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>ISBLANK($G98)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C100">
     <cfRule type="expression" dxfId="4" priority="5">
-      <formula>ISBLANK($G97)</formula>
+      <formula>ISBLANK($G100)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>ISBLANK($G20)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>ISBLANK($G99)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>ISBLANK($G20)</formula>
+  <conditionalFormatting sqref="C101:C106">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>ISBLANK($G101)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C98">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>ISBLANK($G98)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C100:C105">
+  <conditionalFormatting sqref="C29">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ISBLANK($G100)</formula>
+      <formula>ISBLANK($G29)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>